<commit_message>
Update shapes for new version of SHACL-Play
</commit_message>
<xml_diff>
--- a/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
+++ b/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\MASA\01-OpenArchaeo\20-Sources\openarchaeo\federation\src\main\webapp\theme-default\shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77E43B6-85AA-420E-9C4B-F8EBFC7004B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2565CE4B-5310-41B2-AAEC-030962DE8F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14775" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="238">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -151,9 +151,6 @@
     <t>sh:IRI</t>
   </si>
   <si>
-    <t>sh:Warning</t>
-  </si>
-  <si>
     <t>oash:PreferredIdentifier</t>
   </si>
   <si>
@@ -733,13 +730,25 @@
     <t>[ sh:alternativePath (crm:P94_has_created [ sh:inversePath crm:P94i_was_created_by ]) ]</t>
   </si>
   <si>
-    <t>Une création de document DOIT avoir créer 1 et un seul document</t>
-  </si>
-  <si>
     <t>Le P14_carried_out_by sur une création de document DOIT être un E21_Person</t>
   </si>
   <si>
     <t>Le P4_has_time-span sur un E65_Creation DOIT être unique et être un E52_Time-Span.</t>
+  </si>
+  <si>
+    <t>Une création de document DOIT avoir créé 1 et un seul document</t>
+  </si>
+  <si>
+    <t>crm:P94_has_created</t>
+  </si>
+  <si>
+    <t>crm:P94_has_created DOIT n'apparaitre qu'une seule fois et être un crm:E31_Document</t>
+  </si>
+  <si>
+    <t>crm:P8_took_place_on_or_within</t>
+  </si>
+  <si>
+    <t>Le P8_took_place_on_or_within DOIT être unique et être un Site</t>
   </si>
 </sst>
 </file>
@@ -1291,15 +1300,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView windowProtection="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5703125"/>
     <col min="2" max="2" width="27.5703125"/>
-    <col min="3" max="3" width="31.7109375" style="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" style="1"/>
     <col min="5" max="5" width="23.7109375" style="1"/>
     <col min="6" max="6" width="33.140625"/>
@@ -1412,6 +1421,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="11" spans="1:1024" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -1488,359 +1498,319 @@
       <c r="G13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E14" s="1">
         <f>E13+1</f>
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ref="E15:E26" si="0">E14+1</f>
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
         <v>37</v>
       </c>
-      <c r="H15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="16" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
         <v>37</v>
       </c>
-      <c r="H16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
       </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18" t="s">
         <v>37</v>
       </c>
-      <c r="H18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
         <v>37</v>
       </c>
-      <c r="H19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
       </c>
-      <c r="H20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s">
         <v>37</v>
       </c>
-      <c r="H21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
       </c>
-      <c r="H22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
       </c>
-      <c r="H23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
         <v>37</v>
       </c>
-      <c r="H24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
       </c>
-      <c r="H25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
-      </c>
-      <c r="H26" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1860,11 +1830,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ86"/>
+  <dimension ref="A1:AMJ88"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1985,10 +1955,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -2001,7 +1971,7 @@
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -2024,49 +1994,49 @@
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="L12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="N12" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="O12" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AMI12"/>
       <c r="AMJ12"/>
@@ -2076,51 +2046,51 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="G13" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H13" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="I13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="N13" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="O13" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2129,24 +2099,24 @@
         <v>oash:P15</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B15, " sur un ", C15)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15"/>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M15" s="1"/>
     </row>
@@ -2156,87 +2126,87 @@
         <v>oash:P16</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B16, " sur un ", C16)</f>
         <v>Contraintes de crm:P1_is_identified_by sur un oash:Site</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>CONCATENATE("oash:P",ROW(A17))</f>
         <v>oash:P17</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B17, " sur un ", C17)</f>
         <v>Contraintes de skos:prefLabel sur un oash:Site</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1024" ht="63.75" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>CONCATENATE("oash:P",ROW(A18))</f>
         <v>oash:P18</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B18, " sur un ", C18)</f>
         <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18"/>
       <c r="I18" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="N18" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:1024" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2246,14 +2216,14 @@
       </c>
       <c r="C19" s="20"/>
       <c r="F19" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="20"/>
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -2262,20 +2232,20 @@
         <v>oash:P21</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B21, " sur un ", C21)</f>
         <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -2284,33 +2254,33 @@
         <v>1</v>
       </c>
       <c r="N21" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>CONCATENATE("oash:P",ROW(A22))</f>
         <v>oash:P22</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B22, " sur un ", C22)</f>
         <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22"/>
       <c r="I22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
@@ -2319,1141 +2289,1134 @@
         <v>oash:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B23, " sur un ", C23)</f>
         <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G23"/>
       <c r="J23" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>CONCATENATE("oash:P",ROW(A24))</f>
+        <v>oash:P24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
-        <f>CONCATENATE("oash:P",ROW(A25))</f>
-        <v>oash:P25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B25, " sur un ", C25)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25"/>
-      <c r="I25" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>CONCATENATE("oash:P",ROW(A26))</f>
         <v>oash:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B26, " sur un ", C26)</f>
-        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
+        <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G26"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1024" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="str">
+      <c r="I26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
         <f>CONCATENATE("oash:P",ROW(A27))</f>
         <v>oash:P27</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="20" t="str">
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B27, " sur un ", C27)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="I27" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="22"/>
-      <c r="AMJ27" s="18"/>
-    </row>
-    <row r="28" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
+        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1024" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="str">
         <f>CONCATENATE("oash:P",ROW(A28))</f>
         <v>oash:P28</v>
       </c>
-      <c r="B28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="1" t="str">
+      <c r="B28" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="20" t="str">
         <f>CONCATENATE("Contraintes de ", B28, " sur un ", C28)</f>
-        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28"/>
-      <c r="I28" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="I28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="22"/>
+      <c r="AMJ28" s="18"/>
+    </row>
+    <row r="29" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>CONCATENATE("oash:P",ROW(A29))</f>
         <v>oash:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
+        <v>138</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B29, " sur un ", C29)</f>
+        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29"/>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f>CONCATENATE("oash:P",ROW(A30))</f>
+        <v>oash:P30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B30, " sur un ", C30)</f>
         <v>Contraintes de skos:prefLabel sur un oash:Person</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>116</v>
+      </c>
+      <c r="O30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="K29" t="s">
-        <v>117</v>
-      </c>
-      <c r="O29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
-      <c r="A31" t="str">
-        <f>CONCATENATE("oash:P",ROW(A31))</f>
-        <v>oash:P31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B31, " sur un ", C31)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31"/>
-      <c r="I31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>CONCATENATE("oash:P",ROW(A32))</f>
         <v>oash:P32</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>111</v>
+      <c r="B32" t="s">
+        <v>132</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>112</v>
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B32, " sur un ", C32)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>144</v>
+        <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="G32"/>
-      <c r="I32" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>CONCATENATE("oash:P",ROW(A33))</f>
         <v>oash:P33</v>
       </c>
-      <c r="B33" t="s">
-        <v>115</v>
+      <c r="B33" s="21" t="s">
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" t="s">
-        <v>112</v>
+        <v>54</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E33" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B33, " sur un ", C33)</f>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33"/>
+      <c r="I33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>CONCATENATE("oash:P",ROW(A34))</f>
+        <v>oash:P34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B34, " sur un ", C34)</f>
         <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>116</v>
+      </c>
+      <c r="O34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>117</v>
-      </c>
-      <c r="O33" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+    </row>
+    <row r="36" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f t="shared" ref="A36:A41" si="0">CONCATENATE("oash:P",ROW(A36))</f>
+        <v>oash:P36</v>
+      </c>
+      <c r="B36" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <f t="shared" ref="A35:A40" si="0">CONCATENATE("oash:P",ROW(A35))</f>
-        <v>oash:P35</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <f t="shared" ref="E36:E41" si="1">CONCATENATE("Contraintes de ", B36, " sur un ", C36)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="1" t="str">
-        <f t="shared" ref="E35:E40" si="1">CONCATENATE("Contraintes de ", B35, " sur un ", C35)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G35"/>
-      <c r="K35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="str">
+      <c r="G36"/>
+      <c r="K36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>oash:P36</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" s="20" t="str">
+        <v>oash:P37</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F37" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N37" s="19"/>
+    </row>
+    <row r="38" spans="1:15" s="21" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>oash:P38</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I36" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N36" s="19"/>
-    </row>
-    <row r="37" spans="1:15" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P37</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" s="1" t="str">
+      <c r="C38" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A38" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P38</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G38"/>
-      <c r="N38" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>oash:P39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G39"/>
-      <c r="I39" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="N39" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>oash:P40</v>
       </c>
-      <c r="B40" t="s">
-        <v>115</v>
+      <c r="B40" s="21" t="s">
+        <v>154</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G40"/>
+      <c r="I40" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>oash:P41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>116</v>
+      </c>
+      <c r="O41" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>117</v>
-      </c>
-      <c r="O40" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
+    </row>
+    <row r="43" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="str">
+        <f t="shared" ref="A43:A51" si="2">CONCATENATE("oash:P",ROW(A43))</f>
+        <v>oash:P43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <f t="shared" ref="E43:E51" si="3">CONCATENATE("Contraintes de ", B43, " sur un ", C43)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="str">
-        <f t="shared" ref="A42:A50" si="2">CONCATENATE("oash:P",ROW(A42))</f>
-        <v>oash:P42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" s="1" t="str">
-        <f t="shared" ref="E42:E50" si="3">CONCATENATE("Contraintes de ", B42, " sur un ", C42)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G42"/>
-      <c r="K42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P43</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="G43"/>
-      <c r="I43" t="s">
-        <v>40</v>
-      </c>
       <c r="K43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="2"/>
         <v>oash:P44</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G44"/>
-      <c r="N44" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="2"/>
         <v>oash:P45</v>
       </c>
-      <c r="B45" t="s">
-        <v>124</v>
+      <c r="B45" s="21" t="s">
+        <v>152</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="M45" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="str">
+        <v>160</v>
+      </c>
+      <c r="G45"/>
+      <c r="N45" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
         <f t="shared" si="2"/>
         <v>oash:P46</v>
       </c>
-      <c r="B46" s="21" t="s">
-        <v>151</v>
+      <c r="B46" t="s">
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I46" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" s="21" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="str">
         <f t="shared" si="2"/>
         <v>oash:P47</v>
       </c>
-      <c r="B47" t="s">
-        <v>165</v>
+      <c r="B47" s="21" t="s">
+        <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G47"/>
+        <v>163</v>
+      </c>
       <c r="I47" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="str">
         <f t="shared" si="2"/>
         <v>oash:P48</v>
       </c>
-      <c r="B48" s="21" t="s">
-        <v>155</v>
+      <c r="B48" t="s">
+        <v>164</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G48"/>
       <c r="I48" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" si="2"/>
         <v>oash:P49</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crmarch:AP21_contains sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G49"/>
       <c r="I49" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f t="shared" si="2"/>
         <v>oash:P50</v>
       </c>
-      <c r="B50" t="s">
-        <v>115</v>
+      <c r="B50" s="21" t="s">
+        <v>167</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>Contraintes de crmarch:AP21_contains sur un oash:ManMadeFeature</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50"/>
+      <c r="I50" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f t="shared" si="2"/>
+        <v>oash:P51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>116</v>
+      </c>
+      <c r="O51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="K50" t="s">
-        <v>117</v>
-      </c>
-      <c r="O50" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23" t="s">
+    </row>
+    <row r="53" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A53" t="str">
+        <f t="shared" ref="A53:A60" si="4">CONCATENATE("oash:P",ROW(A53))</f>
+        <v>oash:P53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <f t="shared" ref="E53:E60" si="5">CONCATENATE("Contraintes de ", B53, " sur un ", C53)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f t="shared" ref="A52:A59" si="4">CONCATENATE("oash:P",ROW(A52))</f>
-        <v>oash:P52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" s="1" t="str">
-        <f t="shared" ref="E52:E59" si="5">CONCATENATE("Contraintes de ", B52, " sur un ", C52)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G52"/>
-      <c r="K52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A53" t="str">
-        <f t="shared" si="4"/>
-        <v>oash:P53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="G53"/>
-      <c r="I53" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="K53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f t="shared" si="4"/>
         <v>oash:P54</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>153</v>
+      <c r="B54" t="s">
+        <v>113</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G54"/>
-      <c r="N54" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="4"/>
         <v>oash:P55</v>
       </c>
-      <c r="B55" t="s">
-        <v>175</v>
+      <c r="B55" s="21" t="s">
+        <v>152</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G55"/>
       <c r="N55" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f t="shared" si="4"/>
         <v>oash:P56</v>
       </c>
-      <c r="B56" s="21" t="s">
-        <v>111</v>
+      <c r="B56" t="s">
+        <v>174</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>112</v>
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
+        <v>111</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G56"/>
-      <c r="I56" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N56" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f t="shared" si="4"/>
         <v>oash:P57</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G57"/>
-      <c r="I57" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f t="shared" si="4"/>
         <v>oash:P58</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G58"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="I58" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="4"/>
         <v>oash:P59</v>
       </c>
-      <c r="B59" t="s">
-        <v>115</v>
+      <c r="B59" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
-      </c>
-      <c r="D59" t="s">
-        <v>112</v>
+        <v>66</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G59"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A60" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>116</v>
+      </c>
+      <c r="O60" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="K59" t="s">
-        <v>117</v>
-      </c>
-      <c r="O59" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="23" t="s">
+    </row>
+    <row r="62" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A62" t="str">
+        <f t="shared" ref="A62:A68" si="6">CONCATENATE("oash:P",ROW(A62))</f>
+        <v>oash:P62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <f t="shared" ref="E62:E68" si="7">CONCATENATE("Contraintes de ", B62, " sur un ", C62)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicUnit</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A61" t="str">
-        <f t="shared" ref="A61:A67" si="6">CONCATENATE("oash:P",ROW(A61))</f>
-        <v>oash:P61</v>
-      </c>
-      <c r="B61" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" t="s">
-        <v>112</v>
-      </c>
-      <c r="E61" s="1" t="str">
-        <f t="shared" ref="E61:E67" si="7">CONCATENATE("Contraintes de ", B61, " sur un ", C61)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G61"/>
-      <c r="K61" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
-        <f t="shared" si="6"/>
-        <v>oash:P62</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C62" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E62" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G62"/>
-      <c r="I62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="K62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f t="shared" si="6"/>
         <v>oash:P63</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E63" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>186</v>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicUnit</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="G63"/>
-      <c r="M63" s="18"/>
-    </row>
-    <row r="64" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f t="shared" si="6"/>
         <v>oash:P64</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicUnit</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G64"/>
+      <c r="M64" s="18"/>
+    </row>
+    <row r="65" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f t="shared" si="6"/>
         <v>oash:P65</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>111</v>
       </c>
       <c r="E65" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicUnit</v>
+        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicUnit</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G65"/>
+        <v>186</v>
+      </c>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
       <c r="I65" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f t="shared" si="6"/>
         <v>oash:P66</v>
       </c>
-      <c r="B66" t="s">
-        <v>165</v>
+      <c r="B66" s="21" t="s">
+        <v>150</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E66" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicUnit</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicUnit</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G66"/>
-      <c r="I66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I66" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f t="shared" si="6"/>
         <v>oash:P67</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
-      </c>
-      <c r="D67" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="E67" s="1" t="str">
         <f t="shared" si="7"/>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicUnit</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G67"/>
+      <c r="I67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" t="str">
+        <f t="shared" si="6"/>
+        <v>oash:P68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" t="s">
+        <v>111</v>
+      </c>
+      <c r="E68" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>Contraintes de skos:prefLabel sur un oash:StratigraphicUnit</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="O68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="O67" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="23" t="s">
+    </row>
+    <row r="70" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" t="str">
+        <f t="shared" ref="A70:A75" si="8">CONCATENATE("oash:P",ROW(A70))</f>
+        <v>oash:P70</v>
+      </c>
+      <c r="B70" s="13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" t="str">
-        <f>CONCATENATE("oash:P",ROW(A69))</f>
-        <v>oash:P69</v>
-      </c>
-      <c r="B69" s="13" t="s">
+      <c r="C70" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D69" t="s">
-        <v>112</v>
-      </c>
-      <c r="E69" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B69, " sur un ", C69)</f>
-        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G69" s="1">
-        <v>1</v>
-      </c>
-      <c r="H69">
-        <v>1</v>
-      </c>
-      <c r="J69" s="13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A70" t="str">
-        <f>CONCATENATE("oash:P",ROW(A70))</f>
-        <v>oash:P70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>196</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B70, " sur un ", C70)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
+        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -3461,64 +3424,62 @@
       <c r="H70">
         <v>1</v>
       </c>
-      <c r="I70" t="s">
-        <v>76</v>
-      </c>
-      <c r="J70" s="13"/>
-    </row>
-    <row r="71" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="J70" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f>CONCATENATE("oash:P",ROW(A71))</f>
+        <f t="shared" si="8"/>
         <v>oash:P71</v>
       </c>
       <c r="B71" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>75</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E71" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B71, " sur un ", C71)</f>
-        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G71"/>
+        <v>196</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
       <c r="H71">
         <v>1</v>
       </c>
+      <c r="I71" t="s">
+        <v>75</v>
+      </c>
       <c r="J71" s="13"/>
-      <c r="K71" t="s">
-        <v>117</v>
-      </c>
-      <c r="L71" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
-        <f>CONCATENATE("oash:P",ROW(A72))</f>
+        <f t="shared" si="8"/>
         <v>oash:P72</v>
       </c>
       <c r="B72" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E72" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B72, " sur un ", C72)</f>
-        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G72"/>
       <c r="H72">
@@ -3526,309 +3487,366 @@
       </c>
       <c r="J72" s="13"/>
       <c r="K72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L72" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A73" t="str">
+        <f t="shared" si="8"/>
+        <v>oash:P73</v>
+      </c>
+      <c r="B73" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A73" t="str">
-        <f>CONCATENATE("oash:P",ROW(A73))</f>
-        <v>oash:P73</v>
-      </c>
-      <c r="B73" t="s">
-        <v>203</v>
-      </c>
       <c r="C73" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E73" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B73, " sur un ", C73)</f>
-        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="G73"/>
       <c r="H73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="J73" s="13"/>
+      <c r="K73" t="s">
+        <v>116</v>
+      </c>
+      <c r="L73" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
-        <f>CONCATENATE("oash:P",ROW(A74))</f>
+        <f t="shared" si="8"/>
         <v>oash:P74</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" t="s">
+        <v>111</v>
+      </c>
+      <c r="E74" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B74, " sur un ", C74)</f>
+        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A75" t="str">
+        <f t="shared" si="8"/>
+        <v>oash:P75</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G74" s="1">
+      <c r="G75" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="23" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A76" t="str">
-        <f>CONCATENATE("oash:P",ROW(A76))</f>
-        <v>oash:P76</v>
-      </c>
-      <c r="B76" t="s">
-        <v>114</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D76" s="1">
-        <v>1</v>
-      </c>
-      <c r="E76" t="s">
-        <v>44</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G76" s="1">
-        <v>1</v>
-      </c>
-      <c r="I76" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>CONCATENATE("oash:P",ROW(A77))</f>
         <v>oash:P77</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>43</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+      <c r="I77" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" t="str">
+        <f>CONCATENATE("oash:P",ROW(A78))</f>
+        <v>oash:P78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D77" t="s">
-        <v>112</v>
-      </c>
-      <c r="E77" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B77, " sur un ", C77)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
-      </c>
-      <c r="F77" s="1" t="s">
+      <c r="G78"/>
+      <c r="I78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="str">
+        <f t="shared" ref="A79:A84" si="9">CONCATENATE("oash:P",ROW(A79))</f>
+        <v>oash:P79</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" s="1" t="str">
+        <f t="shared" ref="E79" si="10">CONCATENATE("Contraintes de ", B79, " sur un ", C79)</f>
+        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G77"/>
-      <c r="I77" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" t="str">
-        <f t="shared" ref="A78:A82" si="8">CONCATENATE("oash:P",ROW(A78))</f>
-        <v>oash:P78</v>
-      </c>
-      <c r="B78" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D78" t="s">
-        <v>112</v>
-      </c>
-      <c r="E78" s="1" t="str">
-        <f t="shared" ref="E78" si="9">CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="G79"/>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="N79" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="str">
+        <f t="shared" si="9"/>
+        <v>oash:P80</v>
+      </c>
+      <c r="B80" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="G78"/>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="N78" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" t="str">
-        <f t="shared" si="8"/>
-        <v>oash:P79</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="J79" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="N79" s="14"/>
-    </row>
-    <row r="80" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" t="str">
-        <f t="shared" si="8"/>
-        <v>oash:P80</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C80" t="s">
-        <v>227</v>
+      <c r="C80" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G80">
         <v>1</v>
       </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
       <c r="J80" s="13" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="N80" s="14"/>
     </row>
-    <row r="81" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>oash:P81</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="C81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="G81"/>
-      <c r="I81" t="s">
-        <v>52</v>
-      </c>
-      <c r="J81" s="13"/>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>215</v>
+      </c>
       <c r="N81" s="14"/>
     </row>
-    <row r="82" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>oash:P82</v>
       </c>
-      <c r="B82" t="s">
-        <v>196</v>
+      <c r="B82" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>227</v>
-      </c>
-      <c r="D82" t="s">
-        <v>112</v>
-      </c>
-      <c r="E82" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B82, " sur un ", C82)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>234</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="G82"/>
       <c r="H82">
         <v>1</v>
       </c>
-      <c r="I82" t="s">
-        <v>76</v>
+      <c r="I82" s="13" t="s">
+        <v>215</v>
       </c>
       <c r="N82" s="14"/>
     </row>
-    <row r="83" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C83"/>
+    <row r="83" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" t="str">
+        <f t="shared" si="9"/>
+        <v>oash:P83</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" t="s">
+        <v>226</v>
+      </c>
       <c r="E83" s="1"/>
+      <c r="F83" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G83"/>
+      <c r="I83" t="s">
+        <v>51</v>
+      </c>
+      <c r="J83" s="13"/>
       <c r="N83" s="14"/>
     </row>
-    <row r="84" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="23" t="s">
+    <row r="84" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" t="str">
+        <f t="shared" si="9"/>
+        <v>oash:P84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" t="s">
+        <v>226</v>
+      </c>
+      <c r="D84" t="s">
+        <v>111</v>
+      </c>
+      <c r="E84" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B84, " sur un ", C84)</f>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>75</v>
+      </c>
+      <c r="N84" s="14"/>
+    </row>
+    <row r="85" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C85"/>
+      <c r="E85" s="1"/>
+      <c r="N85" s="14"/>
+    </row>
+    <row r="86" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A87" t="str">
+        <f>CONCATENATE("oash:P",ROW(A87))</f>
+        <v>oash:P87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" t="s">
+        <v>111</v>
+      </c>
+      <c r="E87" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B87, " sur un ", C87)</f>
+        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A85" t="str">
-        <f>CONCATENATE("oash:P",ROW(A85))</f>
-        <v>oash:P85</v>
-      </c>
-      <c r="B85" t="s">
-        <v>203</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D85" t="s">
-        <v>112</v>
-      </c>
-      <c r="E85" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B85, " sur un ", C85)</f>
-        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
-      </c>
-      <c r="F85" s="1" t="s">
+      <c r="G87" s="1">
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A88" t="str">
+        <f>CONCATENATE("oash:P",ROW(A88))</f>
+        <v>oash:P88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>202</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" t="s">
+        <v>111</v>
+      </c>
+      <c r="E88" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
+        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G85" s="1">
+      <c r="G88" s="1">
         <v>1</v>
       </c>
-      <c r="K85" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A86" t="str">
-        <f>CONCATENATE("oash:P",ROW(A86))</f>
-        <v>oash:P86</v>
-      </c>
-      <c r="B86" t="s">
-        <v>203</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D86" t="s">
-        <v>112</v>
-      </c>
-      <c r="E86" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B86, " sur un ", C86)</f>
-        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G86" s="1">
-        <v>1</v>
-      </c>
-      <c r="K86" t="s">
-        <v>117</v>
+      <c r="K88" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3838,11 +3856,11 @@
     <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="N18" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="N21" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="N38" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="N44" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="N54" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="N55" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="N78" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
+    <hyperlink ref="N39" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N45" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="N55" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="N56" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="N79" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Update SHACL (A8 -> A2, replace AP21 with P48)
</commit_message>
<xml_diff>
--- a/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
+++ b/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\MASA\01-OpenArchaeo\20-Sources\openarchaeo\federation\src\main\webapp\theme-default\shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2565CE4B-5310-41B2-AAEC-030962DE8F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5366A24-0AB2-4829-97D0-33EDC5F5CB57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14775" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14355" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="238">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -247,18 +247,6 @@
     <t>Il est SOUHAITABLE que les instances de E22_Man-Made_Object soient des IRIs (pas des nœuds anonymes)</t>
   </si>
   <si>
-    <t>oash:StratigraphicUnit</t>
-  </si>
-  <si>
-    <t>crmarch:A8_Stratigraphic_Unit</t>
-  </si>
-  <si>
-    <t>A8 Stratigraphic Unit</t>
-  </si>
-  <si>
-    <t>Il est SOUHAITABLE que les instances de A8_Stratigraphic_Unit soient des IRIs (pas des nœuds anonymes)</t>
-  </si>
-  <si>
     <t>oash:TimeSpanEvent</t>
   </si>
   <si>
@@ -424,12 +412,6 @@
     <t>crmsci:O19_has_found_object</t>
   </si>
   <si>
-    <t>Le O19_has_found_object DOIT être soit un B1_Built_Work, E25_Man-Made_Feature, E22_Man-Made_Object ou A8_Stratigraphic_Unit</t>
-  </si>
-  <si>
-    <t>( [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A8_Stratigraphic_Unit ])</t>
-  </si>
-  <si>
     <t>Contraintes sur les Personnes (E21_Person)</t>
   </si>
   <si>
@@ -535,9 +517,6 @@
     <t>Un P46i_forms_part_of sur un Man-made Feature DOIT être un B1_Built_Work</t>
   </si>
   <si>
-    <t>Un P46_is_composed_of sur un Man-Made Feature DOIT être un A8_Stratigraphic_Unit</t>
-  </si>
-  <si>
     <t>crmarch:AP21_contains</t>
   </si>
   <si>
@@ -574,18 +553,9 @@
     <t>crmarch:AP21i_is_contained_in</t>
   </si>
   <si>
-    <t>Le AP21i_is_contained_in sur un Man-Made Object DOIT être soit un A8_Stratigraphic_Unit soit un E25_Man-Made_Feature</t>
-  </si>
-  <si>
-    <t>( [ sh:class crmarch:A8_Stratigraphic_Unit ] [ sh:class crm:E25_Man-Made_Feature ] )</t>
-  </si>
-  <si>
     <t>Le skos:prefLabel sur un Man-Made Object DOIT être présent</t>
   </si>
   <si>
-    <t>Contraintes sur les Stratigraphic Unit A8_Stratigraphic_Unit)</t>
-  </si>
-  <si>
     <t>Le P3_has_note sur une US DOIT être une valeur litérale.</t>
   </si>
   <si>
@@ -616,12 +586,6 @@
     <t>oash:EncounterEvent, oash:Event</t>
   </si>
   <si>
-    <t>Le P8_took_place_on_or_within ou son inverse P8i_witnessed sur un EncounterEvent ou un Event DOIT être présent, unique, et être soit un Site Built Work, Man-Made Feature, Stratigraphical Unit ou Man-Made Object</t>
-  </si>
-  <si>
-    <t>( [ sh:class crm:E27_Site ] [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A8_Stratigraphic_Unit ])</t>
-  </si>
-  <si>
     <t>crm:P4_has_time-span</t>
   </si>
   <si>
@@ -709,12 +673,6 @@
     <t>crm:P70_documents</t>
   </si>
   <si>
-    <t>Le P70_documents sur un Document DOIT avoir au moins une valeur et être soit un Encounter_Event, soit un Site, soit un Built_Work, soit un Man-Made_Feature, soit une Stratigraphic Unit, soit un Man-Made_Object</t>
-  </si>
-  <si>
-    <t>([ sh:class crmsci:S19_Encounter_Event] [ sh:class crm:E27_Site ] [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A8_Stratigraphic_Unit ])</t>
-  </si>
-  <si>
     <t>oash:DocumentCreation</t>
   </si>
   <si>
@@ -749,6 +707,48 @@
   </si>
   <si>
     <t>Le P8_took_place_on_or_within DOIT être unique et être un Site</t>
+  </si>
+  <si>
+    <t>oash:StratigraphicVolumeUnit</t>
+  </si>
+  <si>
+    <t>crmarch:A2_Stratigraphic_Volume_Unit</t>
+  </si>
+  <si>
+    <t>A2 Stratigraphic Volume Unit</t>
+  </si>
+  <si>
+    <t>Il est SOUHAITABLE que les instances de A2_Stratigraphic_Volume_Unit soient des IRIs (pas des nœuds anonymes)</t>
+  </si>
+  <si>
+    <t>Contraintes sur les Stratigraphic Volume Unit (A2_Stratigraphic_Volume_Unit)</t>
+  </si>
+  <si>
+    <t>Le O19_has_found_object DOIT être soit un B1_Built_Work, E25_Man-Made_Feature, E22_Man-Made_Object ou A2_Stratigraphic_Volume_Unit</t>
+  </si>
+  <si>
+    <t>( [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ])</t>
+  </si>
+  <si>
+    <t>Un P46_is_composed_of sur un Man-Made Feature DOIT être un A2_Stratigraphic_Volume_Unit</t>
+  </si>
+  <si>
+    <t>Le AP21i_is_contained_in sur un Man-Made Object DOIT être une A2_Stratigraphic_Volume_Unit</t>
+  </si>
+  <si>
+    <t>Le P8_took_place_on_or_within ou son inverse P8i_witnessed sur un EncounterEvent ou un Event DOIT être présent, unique, et être soit un Site Built Work, Man-Made Feature, Stratigraphical Volume Unit ou Man-Made Object</t>
+  </si>
+  <si>
+    <t>( [ sh:class crm:E27_Site ] [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ])</t>
+  </si>
+  <si>
+    <t>Le P70_documents sur un Document DOIT avoir au moins une valeur et être soit un Encounter_Event, soit un Site, soit un Built_Work, soit un Man-Made_Feature, soit une Stratigraphic Volume Unit, soit un Man-Made_Object</t>
+  </si>
+  <si>
+    <t>([ sh:class crmsci:S19_Encounter_Event] [ sh:class crm:E27_Site ] [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ])</t>
+  </si>
+  <si>
+    <t>Le P46i_forms_part_of sur un Man-Made Object DOIT être un E25_Man-Made_Feature</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView windowProtection="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1341,7 @@
       <c r="D2" s="3"/>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1695,23 +1695,23 @@
     </row>
     <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
@@ -1719,23 +1719,23 @@
     </row>
     <row r="23" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
@@ -1743,23 +1743,23 @@
     </row>
     <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s">
         <v>37</v>
@@ -1767,23 +1767,23 @@
     </row>
     <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
@@ -1791,23 +1791,23 @@
     </row>
     <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
@@ -1830,11 +1830,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ88"/>
+  <dimension ref="A1:AMJ89"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1955,10 +1955,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -1994,49 +1994,49 @@
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="L12" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>97</v>
-      </c>
       <c r="O12" s="10" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="AMI12"/>
       <c r="AMJ12"/>
@@ -2046,51 +2046,51 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="J13" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2099,20 +2099,20 @@
         <v>oash:P15</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B15, " sur un ", C15)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G15"/>
       <c r="I15" t="s">
@@ -2126,20 +2126,20 @@
         <v>oash:P16</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B16, " sur un ", C16)</f>
         <v>Contraintes de crm:P1_is_identified_by sur un oash:Site</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -2155,29 +2155,29 @@
         <v>oash:P17</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B17, " sur un ", C17)</f>
         <v>Contraintes de skos:prefLabel sur un oash:Site</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O17" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -2186,27 +2186,27 @@
         <v>oash:P18</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B18, " sur un ", C18)</f>
         <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G18"/>
       <c r="I18" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="N18" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:1024" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2216,14 +2216,14 @@
       </c>
       <c r="C19" s="20"/>
       <c r="F19" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G19" s="20"/>
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -2232,20 +2232,20 @@
         <v>oash:P21</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B21, " sur un ", C21)</f>
         <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
@@ -2263,20 +2263,20 @@
         <v>oash:P22</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B22, " sur un ", C22)</f>
         <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G22"/>
       <c r="I22" t="s">
@@ -2289,24 +2289,24 @@
         <v>oash:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B23, " sur un ", C23)</f>
         <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>129</v>
+        <v>229</v>
       </c>
       <c r="G23"/>
       <c r="J23" s="13" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
@@ -2315,14 +2315,14 @@
         <v>oash:P24</v>
       </c>
       <c r="B24" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G24"/>
       <c r="H24">
@@ -2335,7 +2335,7 @@
     </row>
     <row r="25" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -2344,20 +2344,20 @@
         <v>oash:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B26, " sur un ", C26)</f>
         <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G26"/>
       <c r="I26" t="s">
@@ -2371,25 +2371,25 @@
         <v>oash:P27</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B27, " sur un ", C27)</f>
         <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G27"/>
       <c r="I27" s="21"/>
       <c r="J27" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:1024" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
@@ -2398,20 +2398,20 @@
         <v>oash:P28</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E28" s="20" t="str">
         <f>CONCATENATE("Contraintes de ", B28, " sur un ", C28)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G28" s="20"/>
       <c r="I28" s="18" t="s">
@@ -2426,20 +2426,20 @@
         <v>oash:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E29" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B29, " sur un ", C29)</f>
         <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G29"/>
       <c r="I29" t="s">
@@ -2453,34 +2453,34 @@
         <v>oash:P30</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E30" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B30, " sur un ", C30)</f>
         <v>Contraintes de skos:prefLabel sur un oash:Person</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O30" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
@@ -2489,20 +2489,20 @@
         <v>oash:P32</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B32, " sur un ", C32)</f>
         <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G32"/>
       <c r="I32" t="s">
@@ -2515,27 +2515,27 @@
         <v>oash:P33</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>54</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E33" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B33, " sur un ", C33)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G33"/>
       <c r="I33" s="18" t="s">
         <v>39</v>
       </c>
       <c r="N33" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
@@ -2544,34 +2544,34 @@
         <v>oash:P34</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
         <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B34, " sur un ", C34)</f>
         <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O34" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
@@ -2580,24 +2580,24 @@
         <v>oash:P36</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
         <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" ref="E36:E41" si="1">CONCATENATE("Contraintes de ", B36, " sur un ", C36)</f>
         <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G36"/>
       <c r="K36" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
@@ -2606,20 +2606,20 @@
         <v>oash:P37</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E37" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I37" s="18" t="s">
         <v>39</v>
@@ -2632,20 +2632,20 @@
         <v>oash:P38</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>58</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I38" s="21" t="s">
         <v>47</v>
@@ -2657,24 +2657,24 @@
         <v>oash:P39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
         <v>58</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G39"/>
       <c r="N39" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -2683,20 +2683,20 @@
         <v>oash:P40</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
         <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G40"/>
       <c r="I40" s="21" t="s">
@@ -2709,34 +2709,34 @@
         <v>oash:P41</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
         <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="K41" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O41" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -2745,24 +2745,24 @@
         <v>oash:P43</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
         <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" ref="E43:E51" si="3">CONCATENATE("Contraintes de ", B43, " sur un ", C43)</f>
         <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G43"/>
       <c r="K43" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -2771,27 +2771,27 @@
         <v>oash:P44</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
         <v>62</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G44"/>
       <c r="I44" t="s">
         <v>39</v>
       </c>
       <c r="K44" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -2800,24 +2800,24 @@
         <v>oash:P45</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
         <v>62</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G45"/>
       <c r="N45" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -2826,20 +2826,20 @@
         <v>oash:P46</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
         <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="M46" s="13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:15" s="21" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
@@ -2857,20 +2857,20 @@
         <v>oash:P47</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
         <v>62</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I47" s="21" t="s">
         <v>47</v>
@@ -2882,20 +2882,20 @@
         <v>oash:P48</v>
       </c>
       <c r="B48" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C48" t="s">
         <v>62</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G48"/>
       <c r="I48" s="21" t="s">
@@ -2908,24 +2908,24 @@
         <v>oash:P49</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C49" t="s">
         <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>166</v>
+        <v>231</v>
       </c>
       <c r="G49"/>
       <c r="I49" s="21" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -2934,20 +2934,20 @@
         <v>oash:P50</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
         <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de crmarch:AP21_contains sur un oash:ManMadeFeature</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G50"/>
       <c r="I50" s="21" t="s">
@@ -2960,60 +2960,60 @@
         <v>oash:P51</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
         <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O51" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f t="shared" ref="A53:A60" si="4">CONCATENATE("oash:P",ROW(A53))</f>
+        <f t="shared" ref="A53:A61" si="4">CONCATENATE("oash:P",ROW(A53))</f>
         <v>oash:P53</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C53" t="s">
         <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f t="shared" ref="E53:E60" si="5">CONCATENATE("Contraintes de ", B53, " sur un ", C53)</f>
+        <f t="shared" ref="E53:E61" si="5">CONCATENATE("Contraintes de ", B53, " sur un ", C53)</f>
         <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G53"/>
       <c r="K53" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -3022,20 +3022,20 @@
         <v>oash:P54</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
         <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G54"/>
       <c r="I54" t="s">
@@ -3048,24 +3048,24 @@
         <v>oash:P55</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
         <v>66</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G55"/>
       <c r="N55" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -3074,24 +3074,24 @@
         <v>oash:P56</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s">
         <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G56"/>
       <c r="N56" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -3100,20 +3100,20 @@
         <v>oash:P57</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G57"/>
       <c r="I57" t="s">
@@ -3126,20 +3126,20 @@
         <v>oash:P58</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C58" t="s">
         <v>66</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G58"/>
       <c r="I58" s="21" t="s">
@@ -3152,138 +3152,136 @@
         <v>oash:P59</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C59" t="s">
         <v>66</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="G59"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="I59" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f t="shared" si="4"/>
         <v>oash:P60</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
         <v>66</v>
       </c>
-      <c r="D60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" s="1" t="str">
+      <c r="D60" s="21"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G60"/>
+      <c r="I60" t="s">
+        <v>63</v>
+      </c>
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G60">
+      <c r="F61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G61">
         <v>1</v>
       </c>
-      <c r="K60" t="s">
-        <v>116</v>
-      </c>
-      <c r="O60" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
-        <f t="shared" ref="A62:A68" si="6">CONCATENATE("oash:P",ROW(A62))</f>
-        <v>oash:P62</v>
-      </c>
-      <c r="B62" t="s">
-        <v>147</v>
-      </c>
-      <c r="C62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E62" s="1" t="str">
-        <f t="shared" ref="E62:E68" si="7">CONCATENATE("Contraintes de ", B62, " sur un ", C62)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G62"/>
-      <c r="K62" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="K61" t="s">
+        <v>112</v>
+      </c>
+      <c r="O61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="23" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A63:A69" si="6">CONCATENATE("oash:P",ROW(A63))</f>
         <v>oash:P63</v>
       </c>
-      <c r="B63" s="21" t="s">
-        <v>110</v>
+      <c r="B63" t="s">
+        <v>141</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>111</v>
+        <v>224</v>
+      </c>
+      <c r="D63" t="s">
+        <v>107</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicUnit</v>
+        <f t="shared" ref="E63:E69" si="7">CONCATENATE("Contraintes de ", B63, " sur un ", C63)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G63"/>
-      <c r="I63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="K63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f t="shared" si="6"/>
         <v>oash:P64</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D64" t="s">
-        <v>111</v>
+        <v>224</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="E64" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>185</v>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="G64"/>
-      <c r="M64" s="18"/>
+      <c r="I64" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="65" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
@@ -3291,163 +3289,156 @@
         <v>oash:P65</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>224</v>
       </c>
       <c r="D65" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E65" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicUnit</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65"/>
+      <c r="M65" s="18"/>
+    </row>
+    <row r="66" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f t="shared" si="6"/>
         <v>oash:P66</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>111</v>
+        <v>224</v>
+      </c>
+      <c r="D66" t="s">
+        <v>107</v>
       </c>
       <c r="E66" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicUnit</v>
+        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G66"/>
+        <v>176</v>
+      </c>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
       <c r="I66" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f t="shared" si="6"/>
         <v>oash:P67</v>
       </c>
-      <c r="B67" t="s">
-        <v>164</v>
+      <c r="B67" s="21" t="s">
+        <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>224</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E67" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicUnit</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G67"/>
-      <c r="I67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I67" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f t="shared" si="6"/>
         <v>oash:P68</v>
       </c>
       <c r="B68" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" t="s">
-        <v>111</v>
+        <v>224</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="E68" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicUnit</v>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G68">
+        <v>178</v>
+      </c>
+      <c r="G68"/>
+      <c r="I68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" t="str">
+        <f t="shared" si="6"/>
+        <v>oash:P69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G69">
         <v>1</v>
       </c>
-      <c r="O68" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" t="str">
-        <f t="shared" ref="A70:A75" si="8">CONCATENATE("oash:P",ROW(A70))</f>
-        <v>oash:P70</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B70, " sur un ", C70)</f>
-        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G70" s="1">
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
-      </c>
-      <c r="J70" s="13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="O69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A71:A76" si="8">CONCATENATE("oash:P",ROW(A71))</f>
         <v>oash:P71</v>
       </c>
-      <c r="B71" t="s">
-        <v>195</v>
+      <c r="B71" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E71" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B71, " sur un ", C71)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
+        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="G71" s="1">
         <v>1</v>
@@ -3455,43 +3446,41 @@
       <c r="H71">
         <v>1</v>
       </c>
-      <c r="I71" t="s">
-        <v>75</v>
-      </c>
-      <c r="J71" s="13"/>
-    </row>
-    <row r="72" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="J71" s="13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f t="shared" si="8"/>
         <v>oash:P72</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E72" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B72, " sur un ", C72)</f>
-        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G72"/>
+        <v>184</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
       <c r="H72">
         <v>1</v>
       </c>
+      <c r="I72" t="s">
+        <v>71</v>
+      </c>
       <c r="J72" s="13"/>
-      <c r="K72" t="s">
-        <v>116</v>
-      </c>
-      <c r="L72" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="73" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
@@ -3499,20 +3488,20 @@
         <v>oash:P73</v>
       </c>
       <c r="B73" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E73" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B73, " sur un ", C73)</f>
-        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G73"/>
       <c r="H73">
@@ -3520,191 +3509,198 @@
       </c>
       <c r="J73" s="13"/>
       <c r="K73" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L73" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f t="shared" si="8"/>
         <v>oash:P74</v>
       </c>
       <c r="B74" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E74" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B74, " sur un ", C74)</f>
-        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G74"/>
       <c r="H74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="J74" s="13"/>
+      <c r="K74" t="s">
+        <v>112</v>
+      </c>
+      <c r="L74" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f t="shared" si="8"/>
         <v>oash:P75</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>211</v>
+      <c r="B75" t="s">
+        <v>190</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D75" t="s">
+        <v>107</v>
+      </c>
+      <c r="E75" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B75, " sur un ", C75)</f>
+        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G75" s="1">
+        <v>191</v>
+      </c>
+      <c r="G75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A77" t="str">
-        <f>CONCATENATE("oash:P",ROW(A77))</f>
-        <v>oash:P77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>113</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D77" s="1">
+      <c r="H75">
         <v>1</v>
       </c>
-      <c r="E77" t="s">
-        <v>43</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G77" s="1">
+    </row>
+    <row r="76" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f t="shared" si="8"/>
+        <v>oash:P76</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G76" s="1">
         <v>1</v>
       </c>
-      <c r="I77" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
         <f>CONCATENATE("oash:P",ROW(A78))</f>
         <v>oash:P78</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
+        <v>208</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>43</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="str">
+        <f>CONCATENATE("oash:P",ROW(A79))</f>
+        <v>oash:P79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D79" t="s">
+        <v>107</v>
+      </c>
+      <c r="E79" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B79, " sur un ", C79)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G78"/>
-      <c r="I78" t="s">
+      <c r="F79" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G79"/>
+      <c r="I79" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" t="str">
-        <f t="shared" ref="A79:A84" si="9">CONCATENATE("oash:P",ROW(A79))</f>
-        <v>oash:P79</v>
-      </c>
-      <c r="B79" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D79" t="s">
-        <v>111</v>
-      </c>
-      <c r="E79" s="1" t="str">
-        <f t="shared" ref="E79" si="10">CONCATENATE("Contraintes de ", B79, " sur un ", C79)</f>
+    <row r="80" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="str">
+        <f t="shared" ref="A80:A85" si="9">CONCATENATE("oash:P",ROW(A80))</f>
+        <v>oash:P80</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" t="s">
+        <v>107</v>
+      </c>
+      <c r="E80" s="1" t="str">
+        <f t="shared" ref="E80" si="10">CONCATENATE("Contraintes de ", B80, " sur un ", C80)</f>
         <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G79"/>
-      <c r="H79">
+      <c r="F80" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G80"/>
+      <c r="H80">
         <v>1</v>
       </c>
-      <c r="N79" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" t="str">
-        <f t="shared" si="9"/>
-        <v>oash:P80</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G80">
-        <v>1</v>
-      </c>
-      <c r="J80" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="N80" s="14"/>
-    </row>
-    <row r="81" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N80" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f t="shared" si="9"/>
         <v>oash:P81</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C81" t="s">
-        <v>226</v>
+        <v>211</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
-      <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>215</v>
+      <c r="J81" s="13" t="s">
+        <v>236</v>
       </c>
       <c r="N81" s="14"/>
     </row>
@@ -3714,139 +3710,165 @@
         <v>oash:P82</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C82" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G82"/>
+        <v>219</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="N82" s="14"/>
     </row>
-    <row r="83" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f t="shared" si="9"/>
         <v>oash:P83</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="C83" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="G83"/>
-      <c r="I83" t="s">
-        <v>51</v>
-      </c>
-      <c r="J83" s="13"/>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>203</v>
+      </c>
       <c r="N83" s="14"/>
     </row>
-    <row r="84" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
         <f t="shared" si="9"/>
         <v>oash:P84</v>
       </c>
-      <c r="B84" t="s">
-        <v>195</v>
+      <c r="B84" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>226</v>
-      </c>
-      <c r="D84" t="s">
-        <v>111</v>
-      </c>
-      <c r="E84" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B84, " sur un ", C84)</f>
+        <v>212</v>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G84"/>
+      <c r="I84" t="s">
+        <v>51</v>
+      </c>
+      <c r="J84" s="13"/>
+      <c r="N84" s="14"/>
+    </row>
+    <row r="85" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" t="str">
+        <f t="shared" si="9"/>
+        <v>oash:P85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" t="s">
+        <v>212</v>
+      </c>
+      <c r="D85" t="s">
+        <v>107</v>
+      </c>
+      <c r="E85" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B85, " sur un ", C85)</f>
         <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H84">
+      <c r="F85" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H85">
         <v>1</v>
       </c>
-      <c r="I84" t="s">
-        <v>75</v>
-      </c>
-      <c r="N84" s="14"/>
-    </row>
-    <row r="85" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85"/>
-      <c r="E85" s="1"/>
+      <c r="I85" t="s">
+        <v>71</v>
+      </c>
       <c r="N85" s="14"/>
     </row>
-    <row r="86" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="23" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A87" t="str">
-        <f>CONCATENATE("oash:P",ROW(A87))</f>
-        <v>oash:P87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>202</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D87" t="s">
-        <v>111</v>
-      </c>
-      <c r="E87" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B87, " sur un ", C87)</f>
-        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G87" s="1">
-        <v>1</v>
-      </c>
-      <c r="K87" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C86"/>
+      <c r="E86" s="1"/>
+      <c r="N86" s="14"/>
+    </row>
+    <row r="87" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>CONCATENATE("oash:P",ROW(A88))</f>
         <v>oash:P88</v>
       </c>
       <c r="B88" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D88" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E88" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
-        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
+        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
       <c r="K88" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A89" t="str">
+        <f>CONCATENATE("oash:P",ROW(A89))</f>
+        <v>oash:P89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>190</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B89, " sur un ", C89)</f>
+        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G89" s="1">
+        <v>1</v>
+      </c>
+      <c r="K89" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3860,7 +3882,7 @@
     <hyperlink ref="N45" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
     <hyperlink ref="N55" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
     <hyperlink ref="N56" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="N79" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
+    <hyperlink ref="N80" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
New version of shapes
</commit_message>
<xml_diff>
--- a/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
+++ b/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\MASA\01-OpenArchaeo\20-Sources\openarchaeo\federation\src\main\webapp\theme-default\shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA630E-D451-4C93-A033-8E9A8F44A832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC0EA15-7346-45CE-9806-3231E90158EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14355" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="251">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -163,18 +163,6 @@
     <t>Il est SOUHAITABLE que les instances de E42_Identifier soient des IRIs (pas des nœuds anonymes)</t>
   </si>
   <si>
-    <t>oash:Appellation</t>
-  </si>
-  <si>
-    <t>crm:E41_Appellation</t>
-  </si>
-  <si>
-    <t>E41 Appellation</t>
-  </si>
-  <si>
-    <t>Il est SOUHAITABLE que les instances de E41_Appellation soient des IRIs (pas des nœuds anonymes)</t>
-  </si>
-  <si>
     <t>oash:EncounterEvent</t>
   </si>
   <si>
@@ -361,45 +349,27 @@
     <t>sh:Violation</t>
   </si>
   <si>
-    <t>Les P48_has_preferred_identifier sur les Sites DOIVENT être des E42_Identifier</t>
-  </si>
-  <si>
-    <t>crm:P1_is_identified_by</t>
-  </si>
-  <si>
     <t>skos:prefLabel</t>
   </si>
   <si>
-    <t>Le skos:prefLabel sur un Site DOIT être présent</t>
-  </si>
-  <si>
     <t>sh:Literal</t>
   </si>
   <si>
     <t>crm:P53_has_former_or_current_location</t>
   </si>
   <si>
-    <t>Les valeurs de P53_has_former_or_current_location des Sites DOIVENT être des URIs Geonames (sans autre précision)</t>
-  </si>
-  <si>
     <t>crm:E53_Place</t>
   </si>
   <si>
     <t>"^http://sws.geonames.org/(.*)"</t>
   </si>
   <si>
-    <t>Le P87_is_identified_by sur les Places…</t>
-  </si>
-  <si>
     <t>Contraintes sur les Evenements de découverte (S19_Encoutner_Event)</t>
   </si>
   <si>
     <t>crm:P2_has_type</t>
   </si>
   <si>
-    <t>Le P2_has_type sur un évènement de découverte DOIT être présent, unique, et typé avec une et une seule URI des Pactols</t>
-  </si>
-  <si>
     <t>"^https://ark.frantiq.fr/ark:/26678/(.*)"</t>
   </si>
   <si>
@@ -415,24 +385,9 @@
     <t>Contraintes sur les Personnes (E21_Person)</t>
   </si>
   <si>
-    <t>crm:P131_is_identified_by</t>
-  </si>
-  <si>
-    <t>Le P131_is_identified_by sur une Personne DOIT être un E41_Appellation</t>
-  </si>
-  <si>
     <t>crm:P14i_performed</t>
   </si>
   <si>
-    <t>Le P14i_performed sur une Personne DOIT être soit un S19_Encoutner_Event soit un E5_Event</t>
-  </si>
-  <si>
-    <t>( [ sh:class crmsci:S19_Encounter_Event ] [ sh:class crm:E5_Event ] )</t>
-  </si>
-  <si>
-    <t>Le P48_has_preferred_identifier sur une Personne DOIT être un E42_Identifier.</t>
-  </si>
-  <si>
     <t>crm:P107i_is_current_or_former_member_of</t>
   </si>
   <si>
@@ -445,18 +400,12 @@
     <t>Contraintes sur les Institutions  (E40_Legal_Body)</t>
   </si>
   <si>
-    <t>Le P131_is_identified_by sur une Institution DOIT être un E41_Appellation (son nom)</t>
-  </si>
-  <si>
     <t>Le P48_has_preferred_identifier sur une Institution DOIT être un E42_Identifier et DOIT être une URL (l’URL de son site web)</t>
   </si>
   <si>
     <t>"^https?://(.*)"</t>
   </si>
   <si>
-    <t>Le skos:prefLabel sur une Institution DOIT être présent</t>
-  </si>
-  <si>
     <t>Contraintes sur les Built Works (B1_Built_Work)</t>
   </si>
   <si>
@@ -466,15 +415,9 @@
     <t>Le P3_has_note sur un BuiltWork DOIT être une valeur litérale.</t>
   </si>
   <si>
-    <t>Le P48_has_preferred_identifier sur un BuiltWork DOIT être un E42_Identifier</t>
-  </si>
-  <si>
     <t>crmsci:O19i_was_object_found_by</t>
   </si>
   <si>
-    <t>Le O19i_was_object_found_by sur un BuiltWork DOIT être un S19_Encoutner_Event</t>
-  </si>
-  <si>
     <t>crm:P101_had_as_general_use</t>
   </si>
   <si>
@@ -484,9 +427,6 @@
     <t>crm:P46_is_composed_of</t>
   </si>
   <si>
-    <t>Le P46_is_composed_of sur un BuiltWork DOIT être un E25_Man-Made_Feature</t>
-  </si>
-  <si>
     <t>Le skos:prefLabel sur un BuiltWork DOIT être présent</t>
   </si>
   <si>
@@ -496,12 +436,6 @@
     <t>Le P3_has_note sur un Man-Made Feature DOIT être une valeur litérale.</t>
   </si>
   <si>
-    <t>Le P48_has_preferred_identifier sur un Man-Made Feature DOIT être un E42_Identifier.</t>
-  </si>
-  <si>
-    <t>Le P101_had_as_general_use sur un Man-Made Feature DOIT être une URI PACTOLS</t>
-  </si>
-  <si>
     <t>Le P2_has_type sur une Man-Made Feature DOIT être présent, unique et avoir pour valeur soit Feature, Wall ou Burial</t>
   </si>
   <si>
@@ -514,9 +448,6 @@
     <t>crm:P46i_forms_part_of</t>
   </si>
   <si>
-    <t>Un P46i_forms_part_of sur un Man-made Feature DOIT être un B1_Built_Work</t>
-  </si>
-  <si>
     <t>crmarch:AP21_contains</t>
   </si>
   <si>
@@ -529,9 +460,6 @@
     <t>Le P3_has_note sur un Man-Made Object DOIT être une valeur litérale.</t>
   </si>
   <si>
-    <t>Le P1_is_identified_by sur un Man-Made Object DOIT être un E41_Appellation</t>
-  </si>
-  <si>
     <t>Le P101_had_as_general_use sur un Man-Made Object DOIT être une URI PACTOLS</t>
   </si>
   <si>
@@ -550,18 +478,9 @@
     <t>crmarch:AP21i_is_contained_in</t>
   </si>
   <si>
-    <t>Le skos:prefLabel sur un Man-Made Object DOIT être présent</t>
-  </si>
-  <si>
     <t>Le P3_has_note sur une US DOIT être une valeur litérale.</t>
   </si>
   <si>
-    <t>Le P48_has_preferred_identifier sur une US DOIT être un E42_Identifier</t>
-  </si>
-  <si>
-    <t>Le P101_had_as_general_use sur une US DOIT être une des valeurs…</t>
-  </si>
-  <si>
     <t>le AP21_contains sur une US DOIT être un E22_Man-Made_Object</t>
   </si>
   <si>
@@ -571,24 +490,15 @@
     <t>Le P46i_forms_part_of sur une US DOIT être un E25_Man-Made_Feature</t>
   </si>
   <si>
-    <t>Le skos:prefLabel sur une US Object DOIT être présent</t>
-  </si>
-  <si>
     <t>Contraintes sur les Datation (E5_Event et E52_Time-Span)</t>
   </si>
   <si>
     <t>[ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ]</t>
   </si>
   <si>
-    <t>oash:EncounterEvent, oash:Event</t>
-  </si>
-  <si>
     <t>crm:P4_has_time-span</t>
   </si>
   <si>
-    <t>Le P4_has_time-span sur un EncoutnerEvent ou un Event DOIT être présent, unique et être un E52_Time-Span.</t>
-  </si>
-  <si>
     <t>crm:P82a_begin_of_the_begin</t>
   </si>
   <si>
@@ -607,18 +517,9 @@
     <t>rdfs:label</t>
   </si>
   <si>
-    <t>Le rdfs:label sur un TimeSpan DOIT être présent et unique</t>
-  </si>
-  <si>
     <t>Contraintes sur les identifiants et les appellations</t>
   </si>
   <si>
-    <t>Le rdfs:label sur un Preferred Identifier DOIT être présent</t>
-  </si>
-  <si>
-    <t>Le rdfs:label sur une Appellation DOIT être présent</t>
-  </si>
-  <si>
     <t>sh:uniqueLang^^xsd:boolean</t>
   </si>
   <si>
@@ -637,9 +538,6 @@
     <t>Un TimeSpan DOIT avoir au moins un P82a_begin_of_the_begin OU un P82b_end_of_the_end</t>
   </si>
   <si>
-    <t>Le P1_is_identified_by sur un Site DOIT être présent et être un E41_Appellation</t>
-  </si>
-  <si>
     <t>oash:Document</t>
   </si>
   <si>
@@ -655,18 +553,9 @@
     <t>Contraintes sur les Documents E31_Document</t>
   </si>
   <si>
-    <t>Le P1_is_identified_by sur un Document DOIT être présent et être un E41_Appellation</t>
-  </si>
-  <si>
     <t>oash:E31_Document</t>
   </si>
   <si>
-    <t>Les P48_has_preferred_identifier sur les Documents DOIVENT être des E42_Identifier</t>
-  </si>
-  <si>
-    <t>Le P2_has_type sur un Document DOIT être une URI PACTOLS et n'apparait qu'une seule fois</t>
-  </si>
-  <si>
     <t>crm:P70_documents</t>
   </si>
   <si>
@@ -691,9 +580,6 @@
     <t>Le P4_has_time-span sur un E65_Creation DOIT être unique et être un E52_Time-Span.</t>
   </si>
   <si>
-    <t>Une création de document DOIT avoir créé 1 et un seul document</t>
-  </si>
-  <si>
     <t>crm:P94_has_created</t>
   </si>
   <si>
@@ -703,9 +589,6 @@
     <t>crm:P8_took_place_on_or_within</t>
   </si>
   <si>
-    <t>Le P8_took_place_on_or_within DOIT être unique et être un Site</t>
-  </si>
-  <si>
     <t>oash:StratigraphicVolumeUnit</t>
   </si>
   <si>
@@ -730,9 +613,6 @@
     <t>Le AP21i_is_contained_in sur un Man-Made Object DOIT être une A2_Stratigraphic_Volume_Unit</t>
   </si>
   <si>
-    <t>Le P8_took_place_on_or_within ou son inverse P8i_witnessed sur un EncounterEvent ou un Event DOIT être présent, unique, et être soit un Site Built Work, Man-Made Feature, Stratigraphical Volume Unit ou Man-Made Object</t>
-  </si>
-  <si>
     <t>( [ sh:class crm:E27_Site ] [ sh:class crmba:B1_Built_Work ] [ sh:class crm:E25_Man-Made_Feature ] [ sh:class crm:E22_Man-Made_Object ] [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ])</t>
   </si>
   <si>
@@ -749,6 +629,165 @@
   </si>
   <si>
     <t>( [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ] [ sh:class crm:E22_Man-Made_Object ] )</t>
+  </si>
+  <si>
+    <t>Le P3_has_note sur un Site DOIT apparaitre au maximum 1 fois et être un Literal</t>
+  </si>
+  <si>
+    <t>Les valeurs de P53_has_former_or_current_location des Sites DOIVENT être des URIs Geonames (sans autre précision). La propriété DOIT être présente</t>
+  </si>
+  <si>
+    <t>Le P48_has_preferred_identifier sur les Sites DOIT apparaitre au maximum 1 fois et être un E42_Identifier</t>
+  </si>
+  <si>
+    <t>crm:P8i_witnessed</t>
+  </si>
+  <si>
+    <t>Un Site PEUT porter un P8i_witnessed</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crm:P8i_witnessed [ sh:inversePath crm:P8_took_place_on_or_within ]) ]</t>
+  </si>
+  <si>
+    <t>Un Site DOIT être lié à au moins un évènement de découverte S19</t>
+  </si>
+  <si>
+    <t>Le P2_has_type sur un évènement de découverte DOIT être unique, et typé avec une et une seule URI des Pactols</t>
+  </si>
+  <si>
+    <t>Le P48 sur un evènement de découverte doit être unique et être un E42_Identifier</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crm:P14i_performed [ sh:inversePath crm:P14_carried_out_by ]) ]</t>
+  </si>
+  <si>
+    <t>( [ sh:class crmsci:S19_Encounter_Event ] [ sh:class crm:E65_Creation ] )</t>
+  </si>
+  <si>
+    <t>Le P14i_performed sur une Personne DOIT être soit un S19_Encoutner_Event soit un E65_Creation</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crm:P107_has_current_or_former_member [ sh:inversePath crm:P107i_is_current_or_former_member_of ]) ]</t>
+  </si>
+  <si>
+    <t>Un LegalBody DOIT être lié à au moins une Personne</t>
+  </si>
+  <si>
+    <t>Le P48_has_preferred_identifier sur un BuiltWork DOIT exister, être unique, et être un E42_Identifier</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crmsci:O19i_was_object_found_by [ sh:inversePath crmsci:O19_has_found_object ]) ]</t>
+  </si>
+  <si>
+    <t>Le O19i_was_object_found_by sur un BuiltWork PEUT exister</t>
+  </si>
+  <si>
+    <t>Le P46_is_composed_of ou son inverse sur un BuiltWork DOIT être un E25_Man-Made_Feature</t>
+  </si>
+  <si>
+    <t>Le P48_has_preferred_identifier sur un Man-Made Feature DOIT être un E42_Identifier et être unique.</t>
+  </si>
+  <si>
+    <t>Le P101_had_as_general_use sur un Man-Made Feature DOIT être une URI PACTOLS et être unique</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crm:P46i_forms_part_of [ sh:inversePath crm:P46_is_composed_of ]) ]</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crm:P46_is_composed_of [ sh:inversePath crm:P46i_forms_part_of ]) ]</t>
+  </si>
+  <si>
+    <t>Un P46i_forms_part_of sur un Man-made-Feature DOIT être un B1_Built_Work</t>
+  </si>
+  <si>
+    <t>Un P46_is_composed_of ou son inverse P46i sur un Man-Made Feature DOIT être soit un A2_Stratigraphic_Volume_Unit ou un E22_Man-Made_Object</t>
+  </si>
+  <si>
+    <t>[ sh:alternativePath ( crmarch:AP21i_is_contained_in [ sh:inversePath  crmarch:AP21_contains ]) ]</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur une Institution DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur un Site DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur un Man-Made Object DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur une US Object DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le P48_has_preferred_identifier sur une US DOIT être un E42_Identifier et être unique</t>
+  </si>
+  <si>
+    <t>Le P8_took_place_on_or_within DOIT être un Site</t>
+  </si>
+  <si>
+    <t>Le P8_took_place_on_or_within ou son inverse DOIT être unique</t>
+  </si>
+  <si>
+    <t>Une Personne DOIT avoir au moins un P14i ou un ^P14</t>
+  </si>
+  <si>
+    <t>Un BuiltWork DOIT être lié à un et un seul O19i ou l'inverse de O19</t>
+  </si>
+  <si>
+    <t>Un Man-Made Feature DOIT être lié à un et un seul O19i ou inverse de O19</t>
+  </si>
+  <si>
+    <t>Un P46i_forms_part_of ou son inverse P46 sur un Man-made Feature DOIT être unique</t>
+  </si>
+  <si>
+    <t>Un Man-Made Object DOIT être lié à un seul O19i ou inverse de O19</t>
+  </si>
+  <si>
+    <t>Un Man-Made Object DOIT être lié à au maximum 1 AP21i ou inverse de AP21</t>
+  </si>
+  <si>
+    <t>Un Man-Made Object DOIT être lié à au maximum 1 P46i ou inverse de P46</t>
+  </si>
+  <si>
+    <t>Une US DOIT être lié à un et un seul O19i ou inverse de O19 maximum</t>
+  </si>
+  <si>
+    <t>Le P46i_forms_part_of ou son inverse sur une US DOIT être  unique</t>
+  </si>
+  <si>
+    <t>Le P8_took_place_on_or_within ou son inverse P8i_witnessed sur un Event DOIT être présent, unique, et être soit un Site Built Work, Man-Made Feature, Stratigraphical Volume Unit ou Man-Made Object</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur un TimeSpan DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le skos:prefLabel sur un Document DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>Le P2_has_type sur un Document DOIT être une URI PACTOLS</t>
+  </si>
+  <si>
+    <t>Le rdfs:label sur un Preferred Identifier DOIT être présent et unique</t>
+  </si>
+  <si>
+    <t>crm:P94i_was_created_by</t>
+  </si>
+  <si>
+    <t>Un P94i_was_created_by sur un Document doit être un E65_Creation</t>
+  </si>
+  <si>
+    <t>Une création de document DOIT avoir créé au moins 1 document</t>
+  </si>
+  <si>
+    <t>Le P4_has_time-span sur un  Event DOIT être présent, unique et être un E52_Time-Span.</t>
+  </si>
+  <si>
+    <t>Le P4_has_time-span sur un EncoutnerEvent DOIT être unique, mais pas obligatoire et être un E52_Time-Span.</t>
+  </si>
+  <si>
+    <t>( frantiq:pcrtM9HMWQTGJV frantiq:pcrtUu5zfknZ1x frantiq:pcrtcWtmlzv64Z frantiq:pcrt9Xvh4RiNS5 frantiq:pcrt9M0SrAITut )</t>
+  </si>
+  <si>
+    <t>Le P101_had_as_general_use sur une US DOIT être une valeur PACTOLS connue (Construction, Occupation, Destruction, Abandon, Remblais)</t>
   </si>
 </sst>
 </file>
@@ -815,7 +854,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,12 +879,6 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -860,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -903,18 +936,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1298,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView windowProtection="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1555,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1539,7 +1569,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E26" si="0">E14+1</f>
+        <f t="shared" ref="E15:E25" si="0">E14+1</f>
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1549,7 +1579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1604,7 +1634,7 @@
       <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1621,14 +1651,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1671,71 +1701,71 @@
     </row>
     <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>185</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>186</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>187</v>
       </c>
       <c r="G21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>224</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
@@ -1743,23 +1773,23 @@
     </row>
     <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="G24" t="s">
         <v>37</v>
@@ -1767,49 +1797,25 @@
     </row>
     <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>211</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1830,11 +1836,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ88"/>
+  <dimension ref="A1:AMJ98"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="13" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1846,10 +1852,11 @@
     <col min="6" max="6" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37" style="1"/>
     <col min="8" max="8" width="25.42578125"/>
-    <col min="9" max="9" width="16.5703125"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="28.85546875"/>
     <col min="11" max="11" width="20.140625"/>
-    <col min="12" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
     <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="34.85546875" customWidth="1"/>
     <col min="16" max="1025" width="8.5703125"/>
@@ -1955,10 +1962,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -1971,7 +1978,7 @@
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -1994,49 +2001,49 @@
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="L12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K12" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="O12" s="10" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="AMI12"/>
       <c r="AMJ12"/>
@@ -2046,975 +2053,989 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="J13" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>105</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1024" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>CONCATENATE("oash:P",ROW(A15))</f>
+        <f t="shared" ref="A15:A20" si="0">CONCATENATE("oash:P",ROW(A15))</f>
         <v>oash:P15</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B15, " sur un ", C15)</f>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="G15"/>
+      <c r="H15">
+        <v>1</v>
+      </c>
       <c r="I15" t="s">
         <v>39</v>
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:1024" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>CONCATENATE("oash:P",ROW(A16))</f>
+        <f t="shared" si="0"/>
         <v>oash:P16</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B16, " sur un ", C16)</f>
-        <v>Contraintes de crm:P1_is_identified_by sur un oash:Site</v>
+        <v>Contraintes de skos:prefLabel sur un oash:Site</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>CONCATENATE("oash:P",ROW(A17))</f>
+        <f t="shared" si="0"/>
         <v>oash:P17</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B17, " sur un ", C17)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:Site</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1">
+        <v>198</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>CONCATENATE("oash:P",ROW(A18))</f>
+        <f t="shared" si="0"/>
         <v>oash:P18</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B18, " sur un ", C18)</f>
         <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18"/>
-      <c r="I18" s="18" t="s">
-        <v>115</v>
+        <v>199</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="N18" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1024" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="str">
-        <f>CONCATENATE("oash:P",ROW(A19))</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
         <v>oash:P19</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="F19" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="AMJ19"/>
-    </row>
-    <row r="20" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" t="str">
-        <f>CONCATENATE("oash:P",ROW(A21))</f>
-        <v>oash:P21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B21, " sur un ", C21)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="N21" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19"/>
+      <c r="I19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>oash:P20</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>CONCATENATE("oash:P",ROW(A22))</f>
+        <f t="shared" ref="A22:A27" si="1">CONCATENATE("oash:P",ROW(A22))</f>
         <v>oash:P22</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B22, " sur un ", C22)</f>
-        <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
+        <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22"/>
-      <c r="I22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>CONCATENATE("oash:P",ROW(A23))</f>
+        <f t="shared" si="1"/>
         <v>oash:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B23, " sur un ", C23)</f>
+        <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23"/>
+      <c r="I23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
+        <v>oash:P24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B24, " sur un ", C24)</f>
         <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24"/>
+      <c r="J24" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v>oash:P25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G23"/>
-      <c r="J23" s="13" t="s">
+      <c r="G25"/>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f t="shared" si="1"/>
+        <v>oash:P26</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="24" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>CONCATENATE("oash:P",ROW(A24))</f>
-        <v>oash:P24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G24"/>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <f>CONCATENATE("oash:P",ROW(A26))</f>
-        <v>oash:P26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B26, " sur un ", C26)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="G26"/>
-      <c r="I26" t="s">
-        <v>43</v>
+      <c r="H26">
+        <v>1</v>
       </c>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>CONCATENATE("oash:P",ROW(A27))</f>
+        <f t="shared" si="1"/>
         <v>oash:P27</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B27, " sur un ", C27)</f>
-        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>129</v>
+        <v>206</v>
       </c>
       <c r="G27"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1024" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="str">
-        <f>CONCATENATE("oash:P",ROW(A28))</f>
-        <v>oash:P28</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="20" t="str">
-        <f>CONCATENATE("Contraintes de ", B28, " sur un ", C28)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="I28" s="18" t="s">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="AMJ28" s="18"/>
-    </row>
-    <row r="29" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>CONCATENATE("oash:P",ROW(A29))</f>
         <v>oash:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E29" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B29, " sur un ", C29)</f>
-        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
+        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>133</v>
+        <v>209</v>
       </c>
       <c r="G29"/>
-      <c r="I29" t="s">
-        <v>55</v>
-      </c>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="I29" s="18"/>
+      <c r="J29" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>CONCATENATE("oash:P",ROW(A30))</f>
         <v>oash:P30</v>
       </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B30, " sur un ", C30)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:Person</v>
-      </c>
+      <c r="B30" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>134</v>
+        <v>230</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="K30" t="s">
-        <v>112</v>
-      </c>
-      <c r="O30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="I30" s="18"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>CONCATENATE("oash:P",ROW(A31))</f>
+        <v>oash:P31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B31, " sur un ", C31)</f>
+        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31"/>
+      <c r="I31" t="s">
+        <v>51</v>
+      </c>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>CONCATENATE("oash:P",ROW(A32))</f>
         <v>oash:P32</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B32, " sur un ", C32)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
+        <v>Contraintes de skos:prefLabel sur un oash:Person</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G32"/>
-      <c r="I32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <f>CONCATENATE("oash:P",ROW(A33))</f>
-        <v>oash:P33</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B33, " sur un ", C33)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="G33"/>
-      <c r="I33" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>105</v>
+      </c>
+      <c r="O32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>CONCATENATE("oash:P",ROW(A34))</f>
         <v>oash:P34</v>
       </c>
-      <c r="B34" t="s">
-        <v>110</v>
+      <c r="B34" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" t="s">
-        <v>107</v>
+        <v>50</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B34, " sur un ", C34)</f>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f>CONCATENATE("oash:P",ROW(A35))</f>
+        <v>oash:P35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B35, " sur un ", C35)</f>
         <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
-        <v>112</v>
-      </c>
-      <c r="O34" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>105</v>
+      </c>
+      <c r="O35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f t="shared" ref="A36:A41" si="0">CONCATENATE("oash:P",ROW(A36))</f>
+        <f>CONCATENATE("oash:P",ROW(A36))</f>
         <v>oash:P36</v>
       </c>
-      <c r="B36" t="s">
-        <v>141</v>
+      <c r="B36" s="13" t="s">
+        <v>210</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="1" t="str">
-        <f t="shared" ref="E36:E41" si="1">CONCATENATE("Contraintes de ", B36, " sur un ", C36)</f>
+        <v>50</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
+        <f t="shared" ref="A38:A44" si="2">CONCATENATE("oash:P",ROW(A38))</f>
+        <v>oash:P38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <f t="shared" ref="E38:E44" si="3">CONCATENATE("Contraintes de ", B38, " sur un ", C38)</f>
         <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G36"/>
-      <c r="K36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P37</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="20" t="str">
-        <f t="shared" si="1"/>
+      <c r="F38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38"/>
+      <c r="K38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="20" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>oash:P39</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="21" t="str">
+        <f t="shared" si="3"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I37" s="18" t="s">
+      <c r="F39" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" s="20">
+        <v>1</v>
+      </c>
+      <c r="H39" s="20">
+        <v>1</v>
+      </c>
+      <c r="I39" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="N37" s="19"/>
-    </row>
-    <row r="38" spans="1:15" s="21" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P38</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="N39" s="22"/>
+    </row>
+    <row r="40" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>oash:P40</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A39" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P39</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="F40" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>oash:P41</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G41" s="18">
+        <v>1</v>
+      </c>
+      <c r="H41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f t="shared" si="2"/>
+        <v>oash:P42</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G39"/>
-      <c r="N39" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A40" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P40</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G40"/>
-      <c r="I40" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="K41" t="s">
-        <v>112</v>
-      </c>
-      <c r="O41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" ref="A43:A50" si="2">CONCATENATE("oash:P",ROW(A43))</f>
+        <f t="shared" si="2"/>
         <v>oash:P43</v>
       </c>
-      <c r="B43" t="s">
-        <v>141</v>
+      <c r="B43" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f t="shared" ref="E43:E50" si="3">CONCATENATE("Contraintes de ", B43, " sur un ", C43)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
+        <f t="shared" si="3"/>
+        <v>Contraintes de [ sh:alternativePath ( crm:P46_is_composed_of [ sh:inversePath crm:P46i_forms_part_of ]) ] sur un oash:BuiltWork</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>152</v>
+        <v>215</v>
       </c>
       <c r="G43"/>
-      <c r="K43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="I43" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="2"/>
         <v>oash:P44</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>106</v>
+      <c r="B44" t="s">
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>103</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>105</v>
+      </c>
+      <c r="O44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
+        <f t="shared" ref="A46:A56" si="4">CONCATENATE("oash:P",ROW(A46))</f>
+        <v>oash:P46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <f t="shared" ref="E46:E56" si="5">CONCATENATE("Contraintes de ", B46, " sur un ", C46)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46"/>
+      <c r="K46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A47" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P47</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44"/>
-      <c r="I44" t="s">
+      <c r="F47" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="s">
         <v>39</v>
       </c>
-      <c r="K44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A45" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P45</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="K47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A48" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P48</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45"/>
-      <c r="N45" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" t="s">
-        <v>107</v>
-      </c>
-      <c r="E46" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="F48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G48"/>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="N48" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="M46" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" s="21" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P47</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="F49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="M49" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P50</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>158</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G48"/>
-      <c r="I48" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P49</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G49"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="K50" t="s">
-        <v>112</v>
-      </c>
-      <c r="O50" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f t="shared" ref="A52:A60" si="4">CONCATENATE("oash:P",ROW(A52))</f>
+        <v>135</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>oash:P51</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G51" s="18">
+        <v>1</v>
+      </c>
+      <c r="H51" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>oash:P52</v>
       </c>
-      <c r="B52" t="s">
-        <v>141</v>
+      <c r="B52" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" t="s">
-        <v>107</v>
+        <v>58</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f t="shared" ref="E52:E60" si="5">CONCATENATE("Contraintes de ", B52, " sur un ", C52)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
+        <f t="shared" si="5"/>
+        <v>Contraintes de [ sh:alternativePath ( crm:P46i_forms_part_of [ sh:inversePath crm:P46_is_composed_of ]) ] sur un oash:ManMadeFeature</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>163</v>
+        <v>233</v>
       </c>
       <c r="G52"/>
-      <c r="K52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A53" t="str">
+      <c r="H52" s="18">
+        <v>1</v>
+      </c>
+      <c r="I52" s="18"/>
+    </row>
+    <row r="53" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="str">
         <f t="shared" si="4"/>
         <v>oash:P53</v>
       </c>
-      <c r="B53" t="s">
-        <v>109</v>
+      <c r="B53" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D53" s="18"/>
+      <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="G53"/>
-      <c r="I53" t="s">
-        <v>43</v>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -3022,828 +3043,1065 @@
         <f t="shared" si="4"/>
         <v>oash:P54</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>146</v>
+      <c r="B54" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="G54"/>
-      <c r="N54" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="I54" s="18"/>
+      <c r="J54" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="204" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="4"/>
         <v>oash:P55</v>
       </c>
-      <c r="B55" t="s">
-        <v>166</v>
+      <c r="B55" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E55" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
+        <f t="shared" ref="E55" si="6">CONCATENATE("Contraintes de ", B55, " sur un ", C55)</f>
+        <v>Contraintes de [ sh:alternativePath ( crm:P46_is_composed_of [ sh:inversePath crm:P46i_forms_part_of ]) ] sur un oash:ManMadeFeature</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
       <c r="G55"/>
-      <c r="N55" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="I55" s="18"/>
+      <c r="J55" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f t="shared" si="4"/>
         <v>oash:P56</v>
       </c>
-      <c r="B56" s="21" t="s">
-        <v>106</v>
+      <c r="B56" t="s">
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>107</v>
+        <v>58</v>
+      </c>
+      <c r="D56" t="s">
+        <v>103</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
+        <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G56"/>
-      <c r="I56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A57" t="str">
-        <f t="shared" si="4"/>
-        <v>oash:P57</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C57" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E57" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G57"/>
-      <c r="I57" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="K56" t="s">
+        <v>105</v>
+      </c>
+      <c r="O56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A58:A68" si="7">CONCATENATE("oash:P",ROW(A58))</f>
         <v>oash:P58</v>
       </c>
-      <c r="B58" s="21" t="s">
-        <v>170</v>
+      <c r="B58" t="s">
+        <v>124</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>107</v>
+        <v>62</v>
+      </c>
+      <c r="D58" t="s">
+        <v>103</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
+        <f t="shared" ref="E58:E68" si="8">CONCATENATE("Contraintes de ", B58, " sur un ", C58)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>230</v>
+        <v>140</v>
       </c>
       <c r="G58"/>
-      <c r="I58" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="J58" s="13"/>
-    </row>
-    <row r="59" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="K58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>oash:P59</v>
       </c>
-      <c r="B59" t="s">
-        <v>158</v>
+      <c r="B59" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D59" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
+      </c>
       <c r="F59" s="1" t="s">
-        <v>235</v>
+        <v>141</v>
       </c>
       <c r="G59"/>
-      <c r="I59" t="s">
-        <v>63</v>
-      </c>
-      <c r="J59" s="13"/>
+      <c r="N59" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="60" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>oash:P60</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D60" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
+        <f t="shared" si="8"/>
+        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="K60" t="s">
-        <v>112</v>
-      </c>
-      <c r="O60" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="G60"/>
+      <c r="N60" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f t="shared" si="7"/>
+        <v>oash:P61</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G61"/>
+      <c r="I61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f t="shared" ref="A62:A68" si="6">CONCATENATE("oash:P",ROW(A62))</f>
+        <f t="shared" si="7"/>
         <v>oash:P62</v>
       </c>
-      <c r="B62" t="s">
-        <v>141</v>
+      <c r="B62" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>223</v>
-      </c>
-      <c r="D62" t="s">
-        <v>107</v>
+        <v>62</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f t="shared" ref="E62:E68" si="7">CONCATENATE("Contraintes de ", B62, " sur un ", C62)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicVolumeUnit</v>
+        <f t="shared" si="8"/>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="G62"/>
-      <c r="K62" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A63" t="str">
-        <f t="shared" si="6"/>
+      <c r="I62" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A63" s="18" t="str">
+        <f t="shared" si="7"/>
         <v>oash:P63</v>
       </c>
-      <c r="B63" s="21" t="s">
-        <v>106</v>
+      <c r="B63" s="13" t="s">
+        <v>213</v>
       </c>
       <c r="C63" t="s">
-        <v>223</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G63"/>
-      <c r="I63" t="s">
-        <v>39</v>
+        <v>234</v>
+      </c>
+      <c r="H63" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>oash:P64</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="18" t="s">
         <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>223</v>
-      </c>
-      <c r="D64" t="s">
-        <v>107</v>
+        <v>62</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E64" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G64"/>
+      <c r="I64" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J64" s="13"/>
+    </row>
+    <row r="65" spans="1:15" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="G64"/>
-      <c r="M64" s="18"/>
-    </row>
-    <row r="65" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f t="shared" si="6"/>
         <v>oash:P65</v>
       </c>
-      <c r="B65" s="21" t="s">
-        <v>160</v>
+      <c r="B65" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="C65" t="s">
-        <v>223</v>
-      </c>
-      <c r="D65" t="s">
-        <v>107</v>
+        <v>62</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E65" s="1" t="str">
+        <f t="shared" ref="E65" si="9">CONCATENATE("Contraintes de ", B65, " sur un ", C65)</f>
+        <v>Contraintes de [ sh:alternativePath ( crmarch:AP21i_is_contained_in [ sh:inversePath  crmarch:AP21_contains ]) ] sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G65"/>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="13"/>
+    </row>
+    <row r="66" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A66" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A66" t="str">
-        <f t="shared" si="6"/>
         <v>oash:P66</v>
       </c>
-      <c r="B66" s="21" t="s">
-        <v>144</v>
+      <c r="B66" t="s">
+        <v>136</v>
       </c>
       <c r="C66" t="s">
-        <v>223</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E66" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="D66" s="18"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G66"/>
+      <c r="I66" t="s">
+        <v>59</v>
+      </c>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="67" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A67" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G66"/>
-      <c r="I66" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A67" t="str">
-        <f t="shared" si="6"/>
         <v>oash:P67</v>
       </c>
-      <c r="B67" t="s">
-        <v>158</v>
+      <c r="B67" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C67" t="s">
-        <v>223</v>
-      </c>
-      <c r="D67" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E67" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="D67" s="18"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G67"/>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="J67" s="13"/>
+    </row>
+    <row r="68" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A68" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G67"/>
-      <c r="I67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" t="str">
-        <f t="shared" si="6"/>
         <v>oash:P68</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C68" t="s">
-        <v>223</v>
+        <v>62</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E68" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
+        <f t="shared" si="8"/>
+        <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="G68">
         <v>1</v>
       </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>105</v>
+      </c>
       <c r="O68" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
-        <f t="shared" ref="A70:A75" si="8">CONCATENATE("oash:P",ROW(A70))</f>
+        <f t="shared" ref="A70:A78" si="10">CONCATENATE("oash:P",ROW(A70))</f>
         <v>oash:P70</v>
       </c>
-      <c r="B70" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>181</v>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>184</v>
       </c>
       <c r="D70" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E70" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B70, " sur un ", C70)</f>
-        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
+        <f t="shared" ref="E70:E78" si="11">CONCATENATE("Contraintes de ", B70, " sur un ", C70)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G70" s="1">
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
-      </c>
-      <c r="J70" s="13" t="s">
-        <v>232</v>
+        <v>147</v>
+      </c>
+      <c r="G70"/>
+      <c r="K70" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>oash:P71</v>
       </c>
-      <c r="B71" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D71" t="s">
-        <v>107</v>
+      <c r="B71" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E71" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B71, " sur un ", C71)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
+        <f t="shared" si="11"/>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G71" s="1">
-        <v>1</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="G71"/>
       <c r="H71">
         <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>71</v>
-      </c>
-      <c r="J71" s="13"/>
-    </row>
-    <row r="72" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>oash:P72</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" t="s">
         <v>184</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D72" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E72" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B72, " sur un ", C72)</f>
-        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>185</v>
+        <f t="shared" si="11"/>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>250</v>
       </c>
       <c r="G72"/>
-      <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="J72" s="13"/>
-      <c r="K72" t="s">
-        <v>112</v>
-      </c>
-      <c r="L72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="M72" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>oash:P73</v>
       </c>
-      <c r="B73" t="s">
-        <v>187</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>70</v>
+      <c r="B73" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" t="s">
+        <v>184</v>
       </c>
       <c r="D73" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B73, " sur un ", C73)</f>
-        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
+        <f t="shared" si="11"/>
+        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G73"/>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="J73" s="13"/>
-      <c r="K73" t="s">
-        <v>112</v>
-      </c>
-      <c r="L73" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>oash:P74</v>
       </c>
-      <c r="B74" t="s">
-        <v>189</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D74" t="s">
-        <v>107</v>
+      <c r="B74" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" t="s">
+        <v>184</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E74" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B74, " sur un ", C74)</f>
-        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
+        <f t="shared" si="11"/>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="G74"/>
+      <c r="I74" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A75" t="str">
-        <f t="shared" si="8"/>
+      <c r="A75" s="18" t="str">
+        <f t="shared" si="10"/>
         <v>oash:P75</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C75" t="s">
+        <v>184</v>
+      </c>
+      <c r="D75" s="18"/>
+      <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G75" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="23" t="s">
-        <v>205</v>
+        <v>237</v>
+      </c>
+      <c r="G75" s="18">
+        <v>1</v>
+      </c>
+      <c r="H75" s="18">
+        <v>1</v>
+      </c>
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f t="shared" si="10"/>
+        <v>oash:P76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" t="s">
+        <v>184</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E76" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G76"/>
+      <c r="I76" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
-        <f>CONCATENATE("oash:P",ROW(A77))</f>
+        <f t="shared" si="10"/>
         <v>oash:P77</v>
       </c>
-      <c r="B77" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D77" s="1">
-        <v>1</v>
-      </c>
-      <c r="E77" t="s">
-        <v>43</v>
-      </c>
+      <c r="B77" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C77" t="s">
+        <v>184</v>
+      </c>
+      <c r="D77" s="18"/>
+      <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G77" s="1">
-        <v>1</v>
-      </c>
-      <c r="I77" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="G77"/>
+      <c r="H77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
-        <f>CONCATENATE("oash:P",ROW(A78))</f>
+        <f t="shared" si="10"/>
         <v>oash:P78</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>207</v>
+        <v>104</v>
+      </c>
+      <c r="C78" t="s">
+        <v>184</v>
       </c>
       <c r="D78" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
+        <f t="shared" si="11"/>
+        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G78"/>
-      <c r="I78" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" t="str">
-        <f t="shared" ref="A79:A84" si="9">CONCATENATE("oash:P",ROW(A79))</f>
-        <v>oash:P79</v>
-      </c>
-      <c r="B79" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D79" t="s">
-        <v>107</v>
-      </c>
-      <c r="E79" s="1" t="str">
-        <f t="shared" ref="E79" si="10">CONCATENATE("Contraintes de ", B79, " sur un ", C79)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G79"/>
-      <c r="H79">
-        <v>1</v>
-      </c>
-      <c r="N79" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="O78" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="A80:A86" si="12">CONCATENATE("oash:P",ROW(A80))</f>
         <v>oash:P80</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="D80" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B80, " sur un ", C80)</f>
+        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:Event</v>
+      </c>
       <c r="F80" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G80">
+        <v>239</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+      <c r="H80">
         <v>1</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="N80" s="14"/>
-    </row>
-    <row r="81" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>oash:P81</v>
       </c>
-      <c r="B81" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C81" t="s">
-        <v>211</v>
-      </c>
-      <c r="E81" s="1"/>
+      <c r="B81" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" t="s">
+        <v>103</v>
+      </c>
+      <c r="E81" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B81, " sur un ", C81)</f>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:Event</v>
+      </c>
       <c r="F81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G81">
+        <v>247</v>
+      </c>
+      <c r="G81" s="1">
         <v>1</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
-      <c r="I81" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="N81" s="14"/>
-    </row>
-    <row r="82" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I81" t="s">
+        <v>67</v>
+      </c>
+      <c r="J81" s="13"/>
+    </row>
+    <row r="82" spans="1:14" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>oash:P82</v>
       </c>
-      <c r="B82" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C82" t="s">
-        <v>211</v>
-      </c>
-      <c r="E82" s="1"/>
+      <c r="B82" t="s">
+        <v>153</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B82, " sur un ", C82)</f>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent</v>
+      </c>
       <c r="F82" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G82"/>
+        <v>248</v>
+      </c>
       <c r="H82">
         <v>1</v>
       </c>
-      <c r="I82" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="N82" s="14"/>
-    </row>
-    <row r="83" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I82" t="s">
+        <v>67</v>
+      </c>
+      <c r="J82" s="13"/>
+    </row>
+    <row r="83" spans="1:14" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>oash:P83</v>
       </c>
-      <c r="B83" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C83" t="s">
-        <v>211</v>
-      </c>
-      <c r="E83" s="1"/>
+      <c r="B83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B83, " sur un ", C83)</f>
+        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
+      </c>
       <c r="F83" s="1" t="s">
-        <v>216</v>
+        <v>155</v>
       </c>
       <c r="G83"/>
-      <c r="I83" t="s">
-        <v>51</v>
+      <c r="H83">
+        <v>1</v>
       </c>
       <c r="J83" s="13"/>
-      <c r="N83" s="14"/>
-    </row>
-    <row r="84" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K83" t="s">
+        <v>105</v>
+      </c>
+      <c r="L83" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>oash:P84</v>
       </c>
       <c r="B84" t="s">
-        <v>182</v>
-      </c>
-      <c r="C84" t="s">
-        <v>211</v>
+        <v>157</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D84" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E84" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B84, " sur un ", C84)</f>
+        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G84"/>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="J84" s="13"/>
+      <c r="K84" t="s">
+        <v>105</v>
+      </c>
+      <c r="L84" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A85" t="str">
+        <f t="shared" si="12"/>
+        <v>oash:P85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D85" t="s">
+        <v>103</v>
+      </c>
+      <c r="E85" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B85, " sur un ", C85)</f>
+        <v>Contraintes de skos:prefLabel sur un oash:TimeSpanEvent</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A86" t="str">
+        <f t="shared" si="12"/>
+        <v>oash:P86</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" t="str">
+        <f t="shared" ref="A88:A95" si="13">CONCATENATE("oash:P",ROW(A88))</f>
+        <v>oash:P88</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D88" t="s">
+        <v>103</v>
+      </c>
+      <c r="E88" s="1" t="str">
+        <f t="shared" ref="E88" si="14">CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
+        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G88"/>
+      <c r="N88" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P89</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="J89" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="N89" s="14"/>
+    </row>
+    <row r="90" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A90" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>104</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D90" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B90, " sur un ", C90)</f>
+        <v>Contraintes de skos:prefLabel sur un oash:E31_Document</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A91" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G91"/>
+      <c r="I91" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P92</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" t="s">
+        <v>174</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="I92" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="N92" s="14"/>
+    </row>
+    <row r="93" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P93</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" t="s">
+        <v>174</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G93"/>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="N93" s="14"/>
+    </row>
+    <row r="94" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P94</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G94"/>
+      <c r="I94" t="s">
+        <v>47</v>
+      </c>
+      <c r="J94" s="13"/>
+      <c r="N94" s="14"/>
+    </row>
+    <row r="95" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" t="str">
+        <f t="shared" si="13"/>
+        <v>oash:P95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>153</v>
+      </c>
+      <c r="C95" t="s">
+        <v>174</v>
+      </c>
+      <c r="D95" t="s">
+        <v>103</v>
+      </c>
+      <c r="E95" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B95, " sur un ", C95)</f>
         <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84" t="s">
-        <v>71</v>
-      </c>
-      <c r="N84" s="14"/>
-    </row>
-    <row r="85" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85"/>
-      <c r="E85" s="1"/>
-      <c r="N85" s="14"/>
-    </row>
-    <row r="86" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A87" t="str">
-        <f>CONCATENATE("oash:P",ROW(A87))</f>
-        <v>oash:P87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>189</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="F95" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95" t="s">
+        <v>67</v>
+      </c>
+      <c r="N95" s="14"/>
+    </row>
+    <row r="96" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C96"/>
+      <c r="E96" s="1"/>
+      <c r="N96" s="14"/>
+    </row>
+    <row r="97" spans="1:11" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A98" t="str">
+        <f>CONCATENATE("oash:P",ROW(A98))</f>
+        <v>oash:P98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>159</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D87" t="s">
-        <v>107</v>
-      </c>
-      <c r="E87" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B87, " sur un ", C87)</f>
+      <c r="D98" t="s">
+        <v>103</v>
+      </c>
+      <c r="E98" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B98, " sur un ", C98)</f>
         <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G87" s="1">
-        <v>1</v>
-      </c>
-      <c r="K87" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A88" t="str">
-        <f>CONCATENATE("oash:P",ROW(A88))</f>
-        <v>oash:P88</v>
-      </c>
-      <c r="B88" t="s">
-        <v>189</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D88" t="s">
-        <v>107</v>
-      </c>
-      <c r="E88" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
-        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G88" s="1">
-        <v>1</v>
-      </c>
-      <c r="K88" t="s">
-        <v>112</v>
+      <c r="F98" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G98" s="1">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="K98" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3852,12 +4110,12 @@
     <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="N18" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="N21" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="N39" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="N45" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="N54" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="N55" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="N79" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
+    <hyperlink ref="N22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="N42" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N48" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="N59" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="N60" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="N88" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Fix properties on Document
</commit_message>
<xml_diff>
--- a/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
+++ b/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\MASA\01-OpenArchaeo\20-Sources\openarchaeo\federation\src\main\webapp\theme-default\shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC0EA15-7346-45CE-9806-3231E90158EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA61DDF1-506D-4BB2-8CD1-56F468E38C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14355" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="250">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -551,9 +551,6 @@
   </si>
   <si>
     <t>Contraintes sur les Documents E31_Document</t>
-  </si>
-  <si>
-    <t>oash:E31_Document</t>
   </si>
   <si>
     <t>crm:P70_documents</t>
@@ -1701,23 +1698,23 @@
     </row>
     <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G21" t="s">
         <v>37</v>
@@ -1797,23 +1794,23 @@
     </row>
     <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
@@ -1839,8 +1836,8 @@
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="13" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1874,7 +1871,7 @@
       <c r="G1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1888,7 +1885,7 @@
       <c r="G2"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1902,7 +1899,7 @@
       <c r="G3"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +1913,7 @@
       <c r="G4"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1930,7 +1927,7 @@
       <c r="G5"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1943,7 +1940,7 @@
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1957,7 +1954,7 @@
       <c r="G7"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1024" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2119,7 +2116,7 @@
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G15"/>
       <c r="H15">
@@ -2149,7 +2146,7 @@
         <v>Contraintes de skos:prefLabel sur un oash:Site</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -2177,7 +2174,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2205,7 +2202,7 @@
         <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2226,14 +2223,14 @@
         <v>oash:P19</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19"/>
       <c r="I19" s="18" t="s">
@@ -2247,14 +2244,14 @@
         <v>oash:P20</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2288,7 +2285,7 @@
         <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2342,11 +2339,11 @@
         <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G24"/>
       <c r="J24" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2355,14 +2352,14 @@
         <v>oash:P25</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G25"/>
       <c r="I25" t="s">
@@ -2383,7 +2380,7 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G26"/>
       <c r="H26">
@@ -2404,7 +2401,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G27"/>
       <c r="H27">
@@ -2439,12 +2436,12 @@
         <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G29"/>
       <c r="I29" s="18"/>
       <c r="J29" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -2453,14 +2450,14 @@
         <v>oash:P30</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2583,7 +2580,7 @@
         <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2604,14 +2601,14 @@
         <v>oash:P36</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2670,7 +2667,7 @@
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G39" s="20">
         <v>1</v>
@@ -2702,7 +2699,7 @@
         <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I40" s="18" t="s">
         <v>43</v>
@@ -2714,14 +2711,14 @@
         <v>oash:P41</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G41" s="18">
         <v>1</v>
@@ -2765,7 +2762,7 @@
         <v>oash:P43</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C43" t="s">
         <v>54</v>
@@ -2778,7 +2775,7 @@
         <v>Contraintes de [ sh:alternativePath ( crm:P46_is_composed_of [ sh:inversePath crm:P46i_forms_part_of ]) ] sur un oash:BuiltWork</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G43"/>
       <c r="I43" s="18" t="s">
@@ -2869,7 +2866,7 @@
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G47"/>
       <c r="H47">
@@ -2901,7 +2898,7 @@
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G48"/>
       <c r="H48">
@@ -2911,7 +2908,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" si="4"/>
         <v>oash:P49</v>
@@ -2973,14 +2970,14 @@
         <v>oash:P51</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C51" t="s">
         <v>58</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G51" s="18">
         <v>1</v>
@@ -2995,7 +2992,7 @@
         <v>oash:P52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C52" t="s">
         <v>58</v>
@@ -3008,7 +3005,7 @@
         <v>Contraintes de [ sh:alternativePath ( crm:P46i_forms_part_of [ sh:inversePath crm:P46_is_composed_of ]) ] sur un oash:ManMadeFeature</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G52"/>
       <c r="H52" s="18">
@@ -3030,7 +3027,7 @@
       <c r="D53" s="18"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G53"/>
       <c r="H53" s="18"/>
@@ -3057,12 +3054,12 @@
         <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G54"/>
       <c r="I54" s="18"/>
       <c r="J54" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="204" x14ac:dyDescent="0.2">
@@ -3071,7 +3068,7 @@
         <v>oash:P55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C55" t="s">
         <v>58</v>
@@ -3084,12 +3081,12 @@
         <v>Contraintes de [ sh:alternativePath ( crm:P46_is_composed_of [ sh:inversePath crm:P46i_forms_part_of ]) ] sur un oash:ManMadeFeature</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G55"/>
       <c r="I55" s="18"/>
       <c r="J55" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -3267,14 +3264,14 @@
         <v>oash:P63</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C63" t="s">
         <v>62</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H63" s="18">
         <v>1</v>
@@ -3299,11 +3296,11 @@
         <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G64"/>
       <c r="I64" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J64" s="13"/>
     </row>
@@ -3313,7 +3310,7 @@
         <v>oash:P65</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C65" t="s">
         <v>62</v>
@@ -3326,7 +3323,7 @@
         <v>Contraintes de [ sh:alternativePath ( crmarch:AP21i_is_contained_in [ sh:inversePath  crmarch:AP21_contains ]) ] sur un oash:ManMadeObject</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G65"/>
       <c r="H65">
@@ -3349,7 +3346,7 @@
       <c r="D66" s="18"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G66"/>
       <c r="I66" t="s">
@@ -3363,7 +3360,7 @@
         <v>oash:P67</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C67" t="s">
         <v>62</v>
@@ -3371,7 +3368,7 @@
       <c r="D67" s="18"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G67"/>
       <c r="H67">
@@ -3398,7 +3395,7 @@
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -3415,7 +3412,7 @@
     </row>
     <row r="69" spans="1:15" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -3427,7 +3424,7 @@
         <v>124</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D70" t="s">
         <v>103</v>
@@ -3453,7 +3450,7 @@
         <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>103</v>
@@ -3463,7 +3460,7 @@
         <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G71"/>
       <c r="H71">
@@ -3482,7 +3479,7 @@
         <v>127</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D72" t="s">
         <v>103</v>
@@ -3492,11 +3489,11 @@
         <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G72"/>
       <c r="M72" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -3508,7 +3505,7 @@
         <v>137</v>
       </c>
       <c r="C73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D73" t="s">
         <v>103</v>
@@ -3535,7 +3532,7 @@
         <v>126</v>
       </c>
       <c r="C74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>103</v>
@@ -3558,15 +3555,15 @@
         <v>oash:P75</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G75" s="18">
         <v>1</v>
@@ -3585,7 +3582,7 @@
         <v>136</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>103</v>
@@ -3608,15 +3605,15 @@
         <v>oash:P77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C77" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G77"/>
       <c r="H77">
@@ -3632,7 +3629,7 @@
         <v>104</v>
       </c>
       <c r="C78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D78" t="s">
         <v>103</v>
@@ -3642,7 +3639,7 @@
         <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -3674,11 +3671,11 @@
         <v>103</v>
       </c>
       <c r="E80" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B80, " sur un ", C80)</f>
+        <f t="shared" ref="E80:E85" si="13">CONCATENATE("Contraintes de ", B80, " sur un ", C80)</f>
         <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:Event</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G80" s="1">
         <v>1</v>
@@ -3687,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -3705,11 +3702,11 @@
         <v>103</v>
       </c>
       <c r="E81" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B81, " sur un ", C81)</f>
+        <f t="shared" si="13"/>
         <v>Contraintes de crm:P4_has_time-span sur un oash:Event</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G81" s="1">
         <v>1</v>
@@ -3737,11 +3734,11 @@
         <v>103</v>
       </c>
       <c r="E82" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B82, " sur un ", C82)</f>
+        <f t="shared" si="13"/>
         <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -3766,7 +3763,7 @@
         <v>103</v>
       </c>
       <c r="E83" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B83, " sur un ", C83)</f>
+        <f t="shared" si="13"/>
         <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F83" s="1" t="s">
@@ -3799,7 +3796,7 @@
         <v>103</v>
       </c>
       <c r="E84" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B84, " sur un ", C84)</f>
+        <f t="shared" si="13"/>
         <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F84" s="1" t="s">
@@ -3832,11 +3829,11 @@
         <v>103</v>
       </c>
       <c r="E85" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B85, " sur un ", C85)</f>
+        <f t="shared" si="13"/>
         <v>Contraintes de skos:prefLabel sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -3870,24 +3867,24 @@
     </row>
     <row r="88" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
-        <f t="shared" ref="A88:A95" si="13">CONCATENATE("oash:P",ROW(A88))</f>
+        <f t="shared" ref="A88:A95" si="14">CONCATENATE("oash:P",ROW(A88))</f>
         <v>oash:P88</v>
       </c>
       <c r="B88" s="18" t="s">
         <v>110</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D88" t="s">
         <v>103</v>
       </c>
       <c r="E88" s="1" t="str">
-        <f t="shared" ref="E88" si="14">CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
+        <f t="shared" ref="E88" si="15">CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
+        <v>Contraintes de crm:P2_has_type sur un oash:Document</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G88"/>
       <c r="N88" s="14" t="s">
@@ -3896,47 +3893,47 @@
     </row>
     <row r="89" spans="1:14" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P89</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="J89" s="13" t="s">
         <v>193</v>
-      </c>
-      <c r="G89">
-        <v>1</v>
-      </c>
-      <c r="J89" s="13" t="s">
-        <v>194</v>
       </c>
       <c r="N89" s="14"/>
     </row>
     <row r="90" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P90</v>
       </c>
       <c r="B90" t="s">
         <v>104</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D90" t="s">
         <v>103</v>
       </c>
       <c r="E90" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B90, " sur un ", C90)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:E31_Document</v>
+        <v>Contraintes de skos:prefLabel sur un oash:Document</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -3947,38 +3944,38 @@
     </row>
     <row r="91" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P91</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G91"/>
       <c r="I91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P92</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -3990,18 +3987,18 @@
     </row>
     <row r="93" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P93</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G93"/>
       <c r="H93">
@@ -4014,18 +4011,18 @@
     </row>
     <row r="94" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P94</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G94"/>
       <c r="I94" t="s">
@@ -4036,14 +4033,14 @@
     </row>
     <row r="95" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>oash:P95</v>
       </c>
       <c r="B95" t="s">
         <v>153</v>
       </c>
       <c r="C95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D95" t="s">
         <v>103</v>
@@ -4053,7 +4050,7 @@
         <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -4092,7 +4089,7 @@
         <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G98" s="1">
         <v>1</v>

</xml_diff>